<commit_message>
agrego tarea modulo 4 DB
</commit_message>
<xml_diff>
--- a/ENTREGA- Planificacion horas de estudio.xlsx
+++ b/ENTREGA- Planificacion horas de estudio.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\Documents\ARG PROGRAMA\MODULO 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\Documents\ARG_PROGRAMA\MODULO 1\EntregasModulo1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="planificacion hs est.- Bombini" sheetId="4" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -1392,73 +1392,16 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1483,11 +1426,68 @@
     <xf numFmtId="20" fontId="25" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1707,9 +1707,9 @@
   <dimension ref="A1:W1010"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <pane ySplit="16" topLeftCell="A186" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="16" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A3" sqref="A3"/>
-      <selection pane="bottomLeft" activeCell="M188" sqref="M188"/>
+      <selection pane="bottomLeft" activeCell="H94" sqref="H94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.58203125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1737,59 +1737,59 @@
     <row r="1" spans="1:23" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A1" s="3"/>
       <c r="B1" s="33"/>
-      <c r="C1" s="88" t="s">
+      <c r="C1" s="69" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="89"/>
-      <c r="E1" s="89"/>
-      <c r="F1" s="89"/>
-      <c r="G1" s="89"/>
-      <c r="H1" s="89"/>
-      <c r="I1" s="89"/>
-      <c r="J1" s="89"/>
-      <c r="K1" s="89"/>
-      <c r="L1" s="89"/>
-      <c r="M1" s="89"/>
-      <c r="N1" s="89"/>
-      <c r="O1" s="89"/>
-      <c r="P1" s="89"/>
-      <c r="Q1" s="89"/>
-      <c r="R1" s="89"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
+      <c r="H1" s="70"/>
+      <c r="I1" s="70"/>
+      <c r="J1" s="70"/>
+      <c r="K1" s="70"/>
+      <c r="L1" s="70"/>
+      <c r="M1" s="70"/>
+      <c r="N1" s="70"/>
+      <c r="O1" s="70"/>
+      <c r="P1" s="70"/>
+      <c r="Q1" s="70"/>
+      <c r="R1" s="70"/>
     </row>
     <row r="2" spans="1:23" ht="10" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="2"/>
       <c r="B2" s="34"/>
-      <c r="C2" s="92"/>
-      <c r="D2" s="93"/>
-      <c r="E2" s="94" t="s">
+      <c r="C2" s="71"/>
+      <c r="D2" s="72"/>
+      <c r="E2" s="73" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="95"/>
-      <c r="G2" s="95"/>
-      <c r="H2" s="95"/>
-      <c r="I2" s="95"/>
-      <c r="J2" s="95"/>
-      <c r="K2" s="96"/>
-      <c r="L2" s="97" t="s">
+      <c r="F2" s="74"/>
+      <c r="G2" s="74"/>
+      <c r="H2" s="74"/>
+      <c r="I2" s="74"/>
+      <c r="J2" s="74"/>
+      <c r="K2" s="75"/>
+      <c r="L2" s="76" t="s">
         <v>20</v>
       </c>
-      <c r="M2" s="98"/>
-      <c r="N2" s="98"/>
-      <c r="O2" s="98"/>
-      <c r="P2" s="98"/>
-      <c r="Q2" s="98"/>
-      <c r="R2" s="98"/>
-      <c r="S2" s="98"/>
-      <c r="T2" s="98"/>
-      <c r="U2" s="98"/>
-      <c r="V2" s="98"/>
-      <c r="W2" s="99"/>
+      <c r="M2" s="77"/>
+      <c r="N2" s="77"/>
+      <c r="O2" s="77"/>
+      <c r="P2" s="77"/>
+      <c r="Q2" s="77"/>
+      <c r="R2" s="77"/>
+      <c r="S2" s="77"/>
+      <c r="T2" s="77"/>
+      <c r="U2" s="77"/>
+      <c r="V2" s="77"/>
+      <c r="W2" s="78"/>
     </row>
     <row r="3" spans="1:23" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C3" s="100" t="s">
+      <c r="C3" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="101"/>
+      <c r="D3" s="68"/>
       <c r="E3" s="28">
         <v>6</v>
       </c>
@@ -1867,10 +1867,10 @@
       </c>
     </row>
     <row r="4" spans="1:23" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C4" s="100" t="s">
+      <c r="C4" s="67" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="101"/>
+      <c r="D4" s="68"/>
       <c r="E4" s="25"/>
       <c r="F4" s="26"/>
       <c r="G4" s="26"/>
@@ -1900,27 +1900,27 @@
     <row r="5" spans="1:23" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
-      <c r="E5" s="81" t="s">
+      <c r="E5" s="83" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="81"/>
-      <c r="G5" s="81"/>
-      <c r="H5" s="81"/>
-      <c r="I5" s="81"/>
-      <c r="J5" s="81"/>
-      <c r="K5" s="81"/>
-      <c r="L5" s="81"/>
-      <c r="M5" s="81"/>
-      <c r="N5" s="81"/>
-      <c r="O5" s="81"/>
-      <c r="P5" s="81"/>
-      <c r="Q5" s="81"/>
-      <c r="R5" s="81"/>
-      <c r="S5" s="81"/>
-      <c r="T5" s="81"/>
-      <c r="U5" s="81"/>
-      <c r="V5" s="81"/>
-      <c r="W5" s="81"/>
+      <c r="F5" s="83"/>
+      <c r="G5" s="83"/>
+      <c r="H5" s="83"/>
+      <c r="I5" s="83"/>
+      <c r="J5" s="83"/>
+      <c r="K5" s="83"/>
+      <c r="L5" s="83"/>
+      <c r="M5" s="83"/>
+      <c r="N5" s="83"/>
+      <c r="O5" s="83"/>
+      <c r="P5" s="83"/>
+      <c r="Q5" s="83"/>
+      <c r="R5" s="83"/>
+      <c r="S5" s="83"/>
+      <c r="T5" s="83"/>
+      <c r="U5" s="83"/>
+      <c r="V5" s="83"/>
+      <c r="W5" s="83"/>
     </row>
     <row r="6" spans="1:23" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C6" s="9"/>
@@ -1946,12 +1946,12 @@
       <c r="W6" s="6"/>
     </row>
     <row r="7" spans="1:23" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="82" t="s">
+      <c r="C7" s="84" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="83"/>
-      <c r="E7" s="83"/>
-      <c r="F7" s="86">
+      <c r="D7" s="85"/>
+      <c r="E7" s="85"/>
+      <c r="F7" s="88">
         <f>COUNTIF(E4:W4,UPPER("x"))</f>
         <v>3</v>
       </c>
@@ -1967,27 +1967,27 @@
       <c r="P7" s="5"/>
     </row>
     <row r="8" spans="1:23" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C8" s="84"/>
-      <c r="D8" s="85"/>
-      <c r="E8" s="85"/>
-      <c r="F8" s="87"/>
+      <c r="C8" s="86"/>
+      <c r="D8" s="87"/>
+      <c r="E8" s="87"/>
+      <c r="F8" s="89"/>
       <c r="G8" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:23" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:23" ht="12" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C10" s="88" t="s">
+      <c r="C10" s="69" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="89"/>
-      <c r="E10" s="89"/>
-      <c r="F10" s="89"/>
-      <c r="G10" s="89"/>
-      <c r="H10" s="89"/>
-      <c r="I10" s="89"/>
-      <c r="J10" s="89"/>
-      <c r="K10" s="89"/>
+      <c r="D10" s="70"/>
+      <c r="E10" s="70"/>
+      <c r="F10" s="70"/>
+      <c r="G10" s="70"/>
+      <c r="H10" s="70"/>
+      <c r="I10" s="70"/>
+      <c r="J10" s="70"/>
+      <c r="K10" s="70"/>
     </row>
     <row r="11" spans="1:23" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="4"/>
@@ -2047,10 +2047,10 @@
     <row r="13" spans="1:23" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="4"/>
       <c r="B13" s="36"/>
-      <c r="C13" s="73" t="s">
+      <c r="C13" s="92" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="74"/>
+      <c r="D13" s="93"/>
       <c r="E13" s="13" t="s">
         <v>34</v>
       </c>
@@ -2082,10 +2082,10 @@
     <row r="14" spans="1:23" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="4"/>
       <c r="B14" s="36"/>
-      <c r="C14" s="73" t="s">
+      <c r="C14" s="92" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="74"/>
+      <c r="D14" s="93"/>
       <c r="E14" s="14">
         <v>50</v>
       </c>
@@ -2117,10 +2117,10 @@
     <row r="15" spans="1:23" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="4"/>
       <c r="B15" s="36"/>
-      <c r="C15" s="75" t="s">
+      <c r="C15" s="97" t="s">
         <v>21</v>
       </c>
-      <c r="D15" s="76"/>
+      <c r="D15" s="98"/>
       <c r="E15" s="16">
         <v>3</v>
       </c>
@@ -2152,10 +2152,10 @@
     <row r="16" spans="1:23" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
       <c r="B16" s="36"/>
-      <c r="C16" s="73" t="s">
+      <c r="C16" s="92" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="74"/>
+      <c r="D16" s="93"/>
       <c r="E16" s="17">
         <f t="shared" ref="E16:M16" si="1">ROUND(E14/E15,1)</f>
         <v>16.7</v>
@@ -2196,10 +2196,10 @@
     <row r="17" spans="1:16" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A17" s="4"/>
       <c r="B17" s="36"/>
-      <c r="C17" s="77" t="s">
+      <c r="C17" s="99" t="s">
         <v>17</v>
       </c>
-      <c r="D17" s="78"/>
+      <c r="D17" s="100"/>
       <c r="E17" s="19">
         <f t="shared" ref="E17:F17" si="2">E14-SUM(E20:E100)</f>
         <v>2</v>
@@ -2272,7 +2272,7 @@
       <c r="M19" s="24"/>
     </row>
     <row r="20" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="79" t="s">
+      <c r="A20" s="101" t="s">
         <v>45</v>
       </c>
       <c r="B20" s="38" t="s">
@@ -2297,7 +2297,7 @@
       <c r="K20" s="48"/>
       <c r="L20" s="48"/>
       <c r="M20" s="48"/>
-      <c r="N20" s="80" t="s">
+      <c r="N20" s="79" t="s">
         <v>31</v>
       </c>
       <c r="O20">
@@ -2308,7 +2308,7 @@
       </c>
     </row>
     <row r="21" spans="1:16" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="70"/>
+      <c r="A21" s="81"/>
       <c r="B21" s="38" t="s">
         <v>1</v>
       </c>
@@ -2329,7 +2329,7 @@
       <c r="K21" s="51"/>
       <c r="L21" s="51"/>
       <c r="M21" s="51"/>
-      <c r="N21" s="80"/>
+      <c r="N21" s="79"/>
       <c r="O21">
         <v>5</v>
       </c>
@@ -2338,7 +2338,7 @@
       </c>
     </row>
     <row r="22" spans="1:16" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A22" s="70"/>
+      <c r="A22" s="81"/>
       <c r="B22" s="38" t="s">
         <v>2</v>
       </c>
@@ -2361,7 +2361,7 @@
       <c r="K22" s="51"/>
       <c r="L22" s="51"/>
       <c r="M22" s="51"/>
-      <c r="N22" s="80"/>
+      <c r="N22" s="79"/>
       <c r="O22">
         <v>6</v>
       </c>
@@ -2370,7 +2370,7 @@
       </c>
     </row>
     <row r="23" spans="1:16" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A23" s="70"/>
+      <c r="A23" s="81"/>
       <c r="B23" s="38" t="s">
         <v>3</v>
       </c>
@@ -2391,7 +2391,7 @@
       <c r="K23" s="51"/>
       <c r="L23" s="51"/>
       <c r="M23" s="51"/>
-      <c r="N23" s="80"/>
+      <c r="N23" s="79"/>
       <c r="O23">
         <v>7</v>
       </c>
@@ -2400,7 +2400,7 @@
       </c>
     </row>
     <row r="24" spans="1:16" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A24" s="70"/>
+      <c r="A24" s="81"/>
       <c r="B24" s="38" t="s">
         <v>4</v>
       </c>
@@ -2423,7 +2423,7 @@
       <c r="K24" s="51"/>
       <c r="L24" s="51"/>
       <c r="M24" s="51"/>
-      <c r="N24" s="80"/>
+      <c r="N24" s="79"/>
       <c r="O24">
         <v>8</v>
       </c>
@@ -2432,7 +2432,7 @@
       </c>
     </row>
     <row r="25" spans="1:16" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A25" s="70"/>
+      <c r="A25" s="81"/>
       <c r="B25" s="38" t="s">
         <v>5</v>
       </c>
@@ -2455,7 +2455,7 @@
       <c r="K25" s="51"/>
       <c r="L25" s="51"/>
       <c r="M25" s="51"/>
-      <c r="N25" s="80"/>
+      <c r="N25" s="79"/>
       <c r="O25">
         <v>9</v>
       </c>
@@ -2464,7 +2464,7 @@
       </c>
     </row>
     <row r="26" spans="1:16" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A26" s="71"/>
+      <c r="A26" s="82"/>
       <c r="B26" s="40" t="s">
         <v>6</v>
       </c>
@@ -2487,7 +2487,7 @@
       <c r="K26" s="53"/>
       <c r="L26" s="53"/>
       <c r="M26" s="53"/>
-      <c r="N26" s="80"/>
+      <c r="N26" s="79"/>
       <c r="O26">
         <v>10</v>
       </c>
@@ -2496,7 +2496,7 @@
       </c>
     </row>
     <row r="27" spans="1:16" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A27" s="72" t="s">
+      <c r="A27" s="80" t="s">
         <v>23</v>
       </c>
       <c r="B27" s="38" t="s">
@@ -2521,7 +2521,7 @@
       <c r="K27" s="55"/>
       <c r="L27" s="55"/>
       <c r="M27" s="55"/>
-      <c r="N27" s="80"/>
+      <c r="N27" s="79"/>
       <c r="O27">
         <v>11</v>
       </c>
@@ -2530,7 +2530,7 @@
       </c>
     </row>
     <row r="28" spans="1:16" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A28" s="70"/>
+      <c r="A28" s="81"/>
       <c r="B28" s="38" t="s">
         <v>1</v>
       </c>
@@ -2551,7 +2551,7 @@
       <c r="K28" s="51"/>
       <c r="L28" s="51"/>
       <c r="M28" s="51"/>
-      <c r="N28" s="80"/>
+      <c r="N28" s="79"/>
       <c r="O28">
         <v>12</v>
       </c>
@@ -2560,7 +2560,7 @@
       </c>
     </row>
     <row r="29" spans="1:16" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A29" s="70"/>
+      <c r="A29" s="81"/>
       <c r="B29" s="38" t="s">
         <v>2</v>
       </c>
@@ -2583,7 +2583,7 @@
       <c r="K29" s="51"/>
       <c r="L29" s="51"/>
       <c r="M29" s="51"/>
-      <c r="N29" s="80"/>
+      <c r="N29" s="79"/>
       <c r="O29">
         <v>13</v>
       </c>
@@ -2592,7 +2592,7 @@
       </c>
     </row>
     <row r="30" spans="1:16" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A30" s="70"/>
+      <c r="A30" s="81"/>
       <c r="B30" s="38" t="s">
         <v>3</v>
       </c>
@@ -2613,7 +2613,7 @@
       <c r="K30" s="51"/>
       <c r="L30" s="51"/>
       <c r="M30" s="51"/>
-      <c r="N30" s="80"/>
+      <c r="N30" s="79"/>
       <c r="O30">
         <v>14</v>
       </c>
@@ -2622,7 +2622,7 @@
       </c>
     </row>
     <row r="31" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="70"/>
+      <c r="A31" s="81"/>
       <c r="B31" s="38" t="s">
         <v>4</v>
       </c>
@@ -2645,7 +2645,7 @@
       <c r="K31" s="51"/>
       <c r="L31" s="51"/>
       <c r="M31" s="51"/>
-      <c r="N31" s="80"/>
+      <c r="N31" s="79"/>
       <c r="O31">
         <v>15</v>
       </c>
@@ -2654,7 +2654,7 @@
       </c>
     </row>
     <row r="32" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="70"/>
+      <c r="A32" s="81"/>
       <c r="B32" s="38" t="s">
         <v>5</v>
       </c>
@@ -2677,7 +2677,7 @@
       <c r="K32" s="51"/>
       <c r="L32" s="51"/>
       <c r="M32" s="51"/>
-      <c r="N32" s="80"/>
+      <c r="N32" s="79"/>
       <c r="O32">
         <v>16</v>
       </c>
@@ -2686,7 +2686,7 @@
       </c>
     </row>
     <row r="33" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="71"/>
+      <c r="A33" s="82"/>
       <c r="B33" s="40" t="s">
         <v>6</v>
       </c>
@@ -2709,7 +2709,7 @@
       <c r="K33" s="53"/>
       <c r="L33" s="53"/>
       <c r="M33" s="53"/>
-      <c r="N33" s="80"/>
+      <c r="N33" s="79"/>
       <c r="O33">
         <v>17</v>
       </c>
@@ -2718,7 +2718,7 @@
       </c>
     </row>
     <row r="34" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="72" t="s">
+      <c r="A34" s="80" t="s">
         <v>24</v>
       </c>
       <c r="B34" s="38" t="s">
@@ -2743,7 +2743,7 @@
       <c r="K34" s="55"/>
       <c r="L34" s="55"/>
       <c r="M34" s="55"/>
-      <c r="N34" s="80"/>
+      <c r="N34" s="79"/>
       <c r="O34">
         <v>18</v>
       </c>
@@ -2752,7 +2752,7 @@
       </c>
     </row>
     <row r="35" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="70"/>
+      <c r="A35" s="81"/>
       <c r="B35" s="38" t="s">
         <v>1</v>
       </c>
@@ -2775,7 +2775,7 @@
       <c r="K35" s="51"/>
       <c r="L35" s="51"/>
       <c r="M35" s="51"/>
-      <c r="N35" s="80"/>
+      <c r="N35" s="79"/>
       <c r="O35">
         <v>19</v>
       </c>
@@ -2784,7 +2784,7 @@
       </c>
     </row>
     <row r="36" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="70"/>
+      <c r="A36" s="81"/>
       <c r="B36" s="38" t="s">
         <v>2</v>
       </c>
@@ -2807,7 +2807,7 @@
       <c r="K36" s="51"/>
       <c r="L36" s="51"/>
       <c r="M36" s="51"/>
-      <c r="N36" s="80"/>
+      <c r="N36" s="79"/>
       <c r="O36">
         <v>20</v>
       </c>
@@ -2816,7 +2816,7 @@
       </c>
     </row>
     <row r="37" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="70"/>
+      <c r="A37" s="81"/>
       <c r="B37" s="38" t="s">
         <v>3</v>
       </c>
@@ -2839,7 +2839,7 @@
       <c r="K37" s="51"/>
       <c r="L37" s="51"/>
       <c r="M37" s="51"/>
-      <c r="N37" s="80"/>
+      <c r="N37" s="79"/>
       <c r="O37">
         <v>21</v>
       </c>
@@ -2848,7 +2848,7 @@
       </c>
     </row>
     <row r="38" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="70"/>
+      <c r="A38" s="81"/>
       <c r="B38" s="38" t="s">
         <v>4</v>
       </c>
@@ -2871,7 +2871,7 @@
       <c r="K38" s="51"/>
       <c r="L38" s="51"/>
       <c r="M38" s="51"/>
-      <c r="N38" s="80"/>
+      <c r="N38" s="79"/>
       <c r="O38">
         <v>22</v>
       </c>
@@ -2880,7 +2880,7 @@
       </c>
     </row>
     <row r="39" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="70"/>
+      <c r="A39" s="81"/>
       <c r="B39" s="38" t="s">
         <v>5</v>
       </c>
@@ -2903,7 +2903,7 @@
       <c r="K39" s="51"/>
       <c r="L39" s="51"/>
       <c r="M39" s="51"/>
-      <c r="N39" s="80"/>
+      <c r="N39" s="79"/>
       <c r="O39">
         <v>23</v>
       </c>
@@ -2912,7 +2912,7 @@
       </c>
     </row>
     <row r="40" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="71"/>
+      <c r="A40" s="82"/>
       <c r="B40" s="40" t="s">
         <v>6</v>
       </c>
@@ -2935,7 +2935,7 @@
       <c r="K40" s="53"/>
       <c r="L40" s="53"/>
       <c r="M40" s="53"/>
-      <c r="N40" s="80"/>
+      <c r="N40" s="79"/>
       <c r="O40">
         <v>24</v>
       </c>
@@ -2944,7 +2944,7 @@
       </c>
     </row>
     <row r="41" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="72" t="s">
+      <c r="A41" s="80" t="s">
         <v>25</v>
       </c>
       <c r="B41" s="38" t="s">
@@ -2969,7 +2969,7 @@
       <c r="K41" s="55"/>
       <c r="L41" s="55"/>
       <c r="M41" s="55"/>
-      <c r="N41" s="80"/>
+      <c r="N41" s="79"/>
       <c r="O41">
         <v>25</v>
       </c>
@@ -2978,7 +2978,7 @@
       </c>
     </row>
     <row r="42" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="70"/>
+      <c r="A42" s="81"/>
       <c r="B42" s="38" t="s">
         <v>1</v>
       </c>
@@ -3001,7 +3001,7 @@
       <c r="K42" s="51"/>
       <c r="L42" s="51"/>
       <c r="M42" s="51"/>
-      <c r="N42" s="80"/>
+      <c r="N42" s="79"/>
       <c r="O42">
         <v>26</v>
       </c>
@@ -3010,7 +3010,7 @@
       </c>
     </row>
     <row r="43" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="70"/>
+      <c r="A43" s="81"/>
       <c r="B43" s="38" t="s">
         <v>2</v>
       </c>
@@ -3042,7 +3042,7 @@
       </c>
     </row>
     <row r="44" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="70"/>
+      <c r="A44" s="81"/>
       <c r="B44" s="38" t="s">
         <v>3</v>
       </c>
@@ -3074,7 +3074,7 @@
       </c>
     </row>
     <row r="45" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="70"/>
+      <c r="A45" s="81"/>
       <c r="B45" s="38" t="s">
         <v>4</v>
       </c>
@@ -3106,7 +3106,7 @@
       </c>
     </row>
     <row r="46" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="70"/>
+      <c r="A46" s="81"/>
       <c r="B46" s="38" t="s">
         <v>5</v>
       </c>
@@ -3138,7 +3138,7 @@
       </c>
     </row>
     <row r="47" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="71"/>
+      <c r="A47" s="82"/>
       <c r="B47" s="40" t="s">
         <v>6</v>
       </c>
@@ -3170,7 +3170,7 @@
       </c>
     </row>
     <row r="48" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="67" t="s">
+      <c r="A48" s="94" t="s">
         <v>46</v>
       </c>
       <c r="B48" s="38" t="s">
@@ -3204,7 +3204,7 @@
       </c>
     </row>
     <row r="49" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="70"/>
+      <c r="A49" s="81"/>
       <c r="B49" s="38" t="s">
         <v>1</v>
       </c>
@@ -3234,7 +3234,7 @@
       </c>
     </row>
     <row r="50" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="70"/>
+      <c r="A50" s="81"/>
       <c r="B50" s="38" t="s">
         <v>2</v>
       </c>
@@ -3266,7 +3266,7 @@
       </c>
     </row>
     <row r="51" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="70"/>
+      <c r="A51" s="81"/>
       <c r="B51" s="38" t="s">
         <v>3</v>
       </c>
@@ -3296,7 +3296,7 @@
       </c>
     </row>
     <row r="52" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="70"/>
+      <c r="A52" s="81"/>
       <c r="B52" s="38" t="s">
         <v>4</v>
       </c>
@@ -3328,7 +3328,7 @@
       </c>
     </row>
     <row r="53" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="70"/>
+      <c r="A53" s="81"/>
       <c r="B53" s="38" t="s">
         <v>5</v>
       </c>
@@ -3360,7 +3360,7 @@
       </c>
     </row>
     <row r="54" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="71"/>
+      <c r="A54" s="82"/>
       <c r="B54" s="40" t="s">
         <v>6</v>
       </c>
@@ -3392,7 +3392,7 @@
       </c>
     </row>
     <row r="55" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="72" t="s">
+      <c r="A55" s="80" t="s">
         <v>26</v>
       </c>
       <c r="B55" s="38" t="s">
@@ -3426,7 +3426,7 @@
       </c>
     </row>
     <row r="56" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="68"/>
+      <c r="A56" s="95"/>
       <c r="B56" s="38" t="s">
         <v>1</v>
       </c>
@@ -3456,7 +3456,7 @@
       </c>
     </row>
     <row r="57" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="68"/>
+      <c r="A57" s="95"/>
       <c r="B57" s="38" t="s">
         <v>2</v>
       </c>
@@ -3488,7 +3488,7 @@
       </c>
     </row>
     <row r="58" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="68"/>
+      <c r="A58" s="95"/>
       <c r="B58" s="38" t="s">
         <v>3</v>
       </c>
@@ -3518,7 +3518,7 @@
       </c>
     </row>
     <row r="59" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="68"/>
+      <c r="A59" s="95"/>
       <c r="B59" s="38" t="s">
         <v>4</v>
       </c>
@@ -3550,7 +3550,7 @@
       </c>
     </row>
     <row r="60" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="68"/>
+      <c r="A60" s="95"/>
       <c r="B60" s="38" t="s">
         <v>5</v>
       </c>
@@ -3582,7 +3582,7 @@
       </c>
     </row>
     <row r="61" spans="1:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A61" s="69"/>
+      <c r="A61" s="96"/>
       <c r="B61" s="40" t="s">
         <v>6</v>
       </c>
@@ -3614,7 +3614,7 @@
       </c>
     </row>
     <row r="62" spans="1:16" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A62" s="67" t="s">
+      <c r="A62" s="94" t="s">
         <v>39</v>
       </c>
       <c r="B62" s="38" t="s">
@@ -3648,7 +3648,7 @@
       </c>
     </row>
     <row r="63" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="70"/>
+      <c r="A63" s="81"/>
       <c r="B63" s="38" t="s">
         <v>1</v>
       </c>
@@ -3678,7 +3678,7 @@
       </c>
     </row>
     <row r="64" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="70"/>
+      <c r="A64" s="81"/>
       <c r="B64" s="38" t="s">
         <v>2</v>
       </c>
@@ -3710,7 +3710,7 @@
       </c>
     </row>
     <row r="65" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A65" s="70"/>
+      <c r="A65" s="81"/>
       <c r="B65" s="38" t="s">
         <v>3</v>
       </c>
@@ -3740,7 +3740,7 @@
       </c>
     </row>
     <row r="66" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A66" s="70"/>
+      <c r="A66" s="81"/>
       <c r="B66" s="38" t="s">
         <v>4</v>
       </c>
@@ -3772,7 +3772,7 @@
       </c>
     </row>
     <row r="67" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A67" s="70"/>
+      <c r="A67" s="81"/>
       <c r="B67" s="38" t="s">
         <v>5</v>
       </c>
@@ -3806,7 +3806,7 @@
       </c>
     </row>
     <row r="68" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A68" s="71"/>
+      <c r="A68" s="82"/>
       <c r="B68" s="40" t="s">
         <v>6</v>
       </c>
@@ -3838,7 +3838,7 @@
       </c>
     </row>
     <row r="69" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A69" s="67" t="s">
+      <c r="A69" s="94" t="s">
         <v>40</v>
       </c>
       <c r="B69" s="38" t="s">
@@ -3872,7 +3872,7 @@
       </c>
     </row>
     <row r="70" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A70" s="68"/>
+      <c r="A70" s="95"/>
       <c r="B70" s="38" t="s">
         <v>1</v>
       </c>
@@ -3902,7 +3902,7 @@
       </c>
     </row>
     <row r="71" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A71" s="68"/>
+      <c r="A71" s="95"/>
       <c r="B71" s="38" t="s">
         <v>2</v>
       </c>
@@ -3934,7 +3934,7 @@
       </c>
     </row>
     <row r="72" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A72" s="68"/>
+      <c r="A72" s="95"/>
       <c r="B72" s="38" t="s">
         <v>3</v>
       </c>
@@ -3964,7 +3964,7 @@
       </c>
     </row>
     <row r="73" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A73" s="68"/>
+      <c r="A73" s="95"/>
       <c r="B73" s="38" t="s">
         <v>4</v>
       </c>
@@ -3996,7 +3996,7 @@
       </c>
     </row>
     <row r="74" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A74" s="68"/>
+      <c r="A74" s="95"/>
       <c r="B74" s="38" t="s">
         <v>5</v>
       </c>
@@ -4028,7 +4028,7 @@
       </c>
     </row>
     <row r="75" spans="1:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A75" s="69"/>
+      <c r="A75" s="96"/>
       <c r="B75" s="40" t="s">
         <v>6</v>
       </c>
@@ -4060,7 +4060,7 @@
       </c>
     </row>
     <row r="76" spans="1:16" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A76" s="67" t="s">
+      <c r="A76" s="94" t="s">
         <v>44</v>
       </c>
       <c r="B76" s="38" t="s">
@@ -4094,7 +4094,7 @@
       </c>
     </row>
     <row r="77" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A77" s="70"/>
+      <c r="A77" s="81"/>
       <c r="B77" s="38" t="s">
         <v>1</v>
       </c>
@@ -4124,7 +4124,7 @@
       </c>
     </row>
     <row r="78" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A78" s="70"/>
+      <c r="A78" s="81"/>
       <c r="B78" s="38" t="s">
         <v>2</v>
       </c>
@@ -4156,7 +4156,7 @@
       </c>
     </row>
     <row r="79" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A79" s="70"/>
+      <c r="A79" s="81"/>
       <c r="B79" s="38" t="s">
         <v>3</v>
       </c>
@@ -4186,7 +4186,7 @@
       </c>
     </row>
     <row r="80" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A80" s="70"/>
+      <c r="A80" s="81"/>
       <c r="B80" s="38" t="s">
         <v>4</v>
       </c>
@@ -4218,7 +4218,7 @@
       </c>
     </row>
     <row r="81" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A81" s="70"/>
+      <c r="A81" s="81"/>
       <c r="B81" s="38" t="s">
         <v>5</v>
       </c>
@@ -4250,7 +4250,7 @@
       </c>
     </row>
     <row r="82" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A82" s="71"/>
+      <c r="A82" s="82"/>
       <c r="B82" s="40" t="s">
         <v>6</v>
       </c>
@@ -4282,7 +4282,7 @@
       </c>
     </row>
     <row r="83" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A83" s="67" t="s">
+      <c r="A83" s="94" t="s">
         <v>41</v>
       </c>
       <c r="B83" s="38" t="s">
@@ -4316,7 +4316,7 @@
       </c>
     </row>
     <row r="84" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A84" s="68"/>
+      <c r="A84" s="95"/>
       <c r="B84" s="38" t="s">
         <v>1</v>
       </c>
@@ -4346,7 +4346,7 @@
       </c>
     </row>
     <row r="85" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A85" s="68"/>
+      <c r="A85" s="95"/>
       <c r="B85" s="38" t="s">
         <v>2</v>
       </c>
@@ -4378,7 +4378,7 @@
       </c>
     </row>
     <row r="86" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A86" s="68"/>
+      <c r="A86" s="95"/>
       <c r="B86" s="38" t="s">
         <v>3</v>
       </c>
@@ -4408,7 +4408,7 @@
       </c>
     </row>
     <row r="87" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A87" s="68"/>
+      <c r="A87" s="95"/>
       <c r="B87" s="38" t="s">
         <v>4</v>
       </c>
@@ -4440,7 +4440,7 @@
       </c>
     </row>
     <row r="88" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A88" s="68"/>
+      <c r="A88" s="95"/>
       <c r="B88" s="38" t="s">
         <v>5</v>
       </c>
@@ -4450,7 +4450,7 @@
       </c>
       <c r="D88" s="44">
         <f t="shared" si="8"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E88" s="50"/>
       <c r="F88" s="51"/>
@@ -4458,7 +4458,7 @@
         <v>3</v>
       </c>
       <c r="H88" s="51">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I88" s="51"/>
       <c r="J88" s="51"/>
@@ -4474,7 +4474,7 @@
       </c>
     </row>
     <row r="89" spans="1:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A89" s="69"/>
+      <c r="A89" s="96"/>
       <c r="B89" s="40" t="s">
         <v>6</v>
       </c>
@@ -4506,7 +4506,7 @@
       </c>
     </row>
     <row r="90" spans="1:16" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A90" s="67" t="s">
+      <c r="A90" s="94" t="s">
         <v>42</v>
       </c>
       <c r="B90" s="38" t="s">
@@ -4540,7 +4540,7 @@
       </c>
     </row>
     <row r="91" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A91" s="70"/>
+      <c r="A91" s="81"/>
       <c r="B91" s="38" t="s">
         <v>1</v>
       </c>
@@ -4550,13 +4550,13 @@
       </c>
       <c r="D91" s="44">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E91" s="50"/>
       <c r="F91" s="51"/>
       <c r="G91" s="51"/>
       <c r="H91" s="51">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I91" s="51"/>
       <c r="J91" s="51"/>
@@ -4572,7 +4572,7 @@
       </c>
     </row>
     <row r="92" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A92" s="70"/>
+      <c r="A92" s="81"/>
       <c r="B92" s="38" t="s">
         <v>2</v>
       </c>
@@ -4604,7 +4604,7 @@
       </c>
     </row>
     <row r="93" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A93" s="70"/>
+      <c r="A93" s="81"/>
       <c r="B93" s="38" t="s">
         <v>3</v>
       </c>
@@ -4614,13 +4614,13 @@
       </c>
       <c r="D93" s="44">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E93" s="50"/>
       <c r="F93" s="51"/>
       <c r="G93" s="51"/>
       <c r="H93" s="51">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I93" s="51"/>
       <c r="J93" s="51"/>
@@ -4636,7 +4636,7 @@
       </c>
     </row>
     <row r="94" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A94" s="70"/>
+      <c r="A94" s="81"/>
       <c r="B94" s="38" t="s">
         <v>4</v>
       </c>
@@ -4646,13 +4646,13 @@
       </c>
       <c r="D94" s="44">
         <f t="shared" si="10"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E94" s="50"/>
       <c r="F94" s="51"/>
       <c r="G94" s="51"/>
       <c r="H94" s="51">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I94" s="51"/>
       <c r="J94" s="51"/>
@@ -4668,7 +4668,7 @@
       </c>
     </row>
     <row r="95" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A95" s="70"/>
+      <c r="A95" s="81"/>
       <c r="B95" s="38" t="s">
         <v>5</v>
       </c>
@@ -4678,13 +4678,13 @@
       </c>
       <c r="D95" s="44">
         <f t="shared" si="10"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E95" s="50"/>
       <c r="F95" s="51"/>
       <c r="G95" s="51"/>
       <c r="H95" s="51">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I95" s="51"/>
       <c r="J95" s="51"/>
@@ -4700,7 +4700,7 @@
       </c>
     </row>
     <row r="96" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A96" s="71"/>
+      <c r="A96" s="82"/>
       <c r="B96" s="40" t="s">
         <v>6</v>
       </c>
@@ -4732,7 +4732,7 @@
       </c>
     </row>
     <row r="97" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A97" s="67" t="s">
+      <c r="A97" s="94" t="s">
         <v>43</v>
       </c>
       <c r="B97" s="38" t="s">
@@ -4766,7 +4766,7 @@
       </c>
     </row>
     <row r="98" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A98" s="68"/>
+      <c r="A98" s="95"/>
       <c r="B98" s="38" t="s">
         <v>1</v>
       </c>
@@ -4776,12 +4776,14 @@
       </c>
       <c r="D98" s="44">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E98" s="50"/>
       <c r="F98" s="51"/>
       <c r="G98" s="51"/>
-      <c r="H98" s="51"/>
+      <c r="H98" s="51">
+        <v>2</v>
+      </c>
       <c r="I98" s="51"/>
       <c r="J98" s="51"/>
       <c r="K98" s="51"/>
@@ -4796,7 +4798,7 @@
       </c>
     </row>
     <row r="99" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A99" s="68"/>
+      <c r="A99" s="95"/>
       <c r="B99" s="38" t="s">
         <v>2</v>
       </c>
@@ -4828,7 +4830,7 @@
       </c>
     </row>
     <row r="100" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A100" s="68"/>
+      <c r="A100" s="95"/>
       <c r="B100" s="38" t="s">
         <v>3</v>
       </c>
@@ -4838,12 +4840,14 @@
       </c>
       <c r="D100" s="44">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E100" s="50"/>
       <c r="F100" s="51"/>
       <c r="G100" s="51"/>
-      <c r="H100" s="51"/>
+      <c r="H100" s="51">
+        <v>2</v>
+      </c>
       <c r="I100" s="51"/>
       <c r="J100" s="51"/>
       <c r="K100" s="51"/>
@@ -4858,7 +4862,7 @@
       </c>
     </row>
     <row r="101" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A101" s="68"/>
+      <c r="A101" s="95"/>
       <c r="B101" s="38" t="s">
         <v>4</v>
       </c>
@@ -4868,13 +4872,13 @@
       </c>
       <c r="D101" s="44">
         <f t="shared" si="10"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E101" s="50"/>
       <c r="F101" s="51"/>
       <c r="G101" s="51"/>
       <c r="H101" s="51">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I101" s="51"/>
       <c r="J101" s="51"/>
@@ -4890,7 +4894,7 @@
       </c>
     </row>
     <row r="102" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A102" s="68"/>
+      <c r="A102" s="95"/>
       <c r="B102" s="38" t="s">
         <v>5</v>
       </c>
@@ -4900,15 +4904,17 @@
       </c>
       <c r="D102" s="44">
         <f t="shared" si="10"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E102" s="50"/>
       <c r="F102" s="51"/>
       <c r="G102" s="51"/>
       <c r="H102" s="51">
-        <v>4</v>
-      </c>
-      <c r="I102" s="51"/>
+        <v>5</v>
+      </c>
+      <c r="I102" s="51">
+        <v>3</v>
+      </c>
       <c r="J102" s="51"/>
       <c r="K102" s="51"/>
       <c r="L102" s="51"/>
@@ -4922,7 +4928,7 @@
       </c>
     </row>
     <row r="103" spans="1:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A103" s="69"/>
+      <c r="A103" s="96"/>
       <c r="B103" s="40" t="s">
         <v>6</v>
       </c>
@@ -4937,10 +4943,10 @@
       <c r="E103" s="58"/>
       <c r="F103" s="59"/>
       <c r="G103" s="59"/>
-      <c r="H103" s="59">
-        <v>5</v>
-      </c>
-      <c r="I103" s="59"/>
+      <c r="H103" s="59"/>
+      <c r="I103" s="59">
+        <v>5</v>
+      </c>
       <c r="J103" s="59"/>
       <c r="K103" s="59"/>
       <c r="L103" s="59"/>
@@ -4954,7 +4960,7 @@
       </c>
     </row>
     <row r="104" spans="1:16" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A104" s="67" t="s">
+      <c r="A104" s="94" t="s">
         <v>47</v>
       </c>
       <c r="B104" s="38" t="s">
@@ -4971,10 +4977,10 @@
       <c r="E104" s="56"/>
       <c r="F104" s="57"/>
       <c r="G104" s="57"/>
-      <c r="H104" s="57">
+      <c r="H104" s="57"/>
+      <c r="I104" s="57">
         <v>2</v>
       </c>
-      <c r="I104" s="57"/>
       <c r="J104" s="57"/>
       <c r="K104" s="57"/>
       <c r="L104" s="57"/>
@@ -4988,7 +4994,7 @@
       </c>
     </row>
     <row r="105" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A105" s="68"/>
+      <c r="A105" s="95"/>
       <c r="B105" s="38" t="s">
         <v>1</v>
       </c>
@@ -4998,15 +5004,15 @@
       </c>
       <c r="D105" s="44">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E105" s="50"/>
       <c r="F105" s="51"/>
       <c r="G105" s="51"/>
-      <c r="H105" s="51">
-        <v>1</v>
-      </c>
-      <c r="I105" s="51"/>
+      <c r="H105" s="51"/>
+      <c r="I105" s="51">
+        <v>2</v>
+      </c>
       <c r="J105" s="51"/>
       <c r="K105" s="51"/>
       <c r="L105" s="51"/>
@@ -5020,7 +5026,7 @@
       </c>
     </row>
     <row r="106" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A106" s="68"/>
+      <c r="A106" s="95"/>
       <c r="B106" s="38" t="s">
         <v>2</v>
       </c>
@@ -5035,10 +5041,10 @@
       <c r="E106" s="50"/>
       <c r="F106" s="51"/>
       <c r="G106" s="51"/>
-      <c r="H106" s="51">
-        <v>3</v>
-      </c>
-      <c r="I106" s="51"/>
+      <c r="H106" s="51"/>
+      <c r="I106" s="51">
+        <v>3</v>
+      </c>
       <c r="J106" s="51"/>
       <c r="K106" s="51"/>
       <c r="L106" s="51"/>
@@ -5052,7 +5058,7 @@
       </c>
     </row>
     <row r="107" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A107" s="68"/>
+      <c r="A107" s="95"/>
       <c r="B107" s="38" t="s">
         <v>3</v>
       </c>
@@ -5062,15 +5068,15 @@
       </c>
       <c r="D107" s="44">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E107" s="50"/>
       <c r="F107" s="51"/>
       <c r="G107" s="51"/>
-      <c r="H107" s="51">
-        <v>1</v>
-      </c>
-      <c r="I107" s="51"/>
+      <c r="H107" s="51"/>
+      <c r="I107" s="51">
+        <v>3</v>
+      </c>
       <c r="J107" s="51"/>
       <c r="K107" s="51"/>
       <c r="L107" s="51"/>
@@ -5084,7 +5090,7 @@
       </c>
     </row>
     <row r="108" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A108" s="68"/>
+      <c r="A108" s="95"/>
       <c r="B108" s="38" t="s">
         <v>4</v>
       </c>
@@ -5116,7 +5122,7 @@
       </c>
     </row>
     <row r="109" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A109" s="68"/>
+      <c r="A109" s="95"/>
       <c r="B109" s="38" t="s">
         <v>5</v>
       </c>
@@ -5126,14 +5132,14 @@
       </c>
       <c r="D109" s="44">
         <f t="shared" si="12"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E109" s="50"/>
       <c r="F109" s="51"/>
       <c r="G109" s="51"/>
       <c r="H109" s="51"/>
       <c r="I109" s="51">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J109" s="51"/>
       <c r="K109" s="51"/>
@@ -5148,7 +5154,7 @@
       </c>
     </row>
     <row r="110" spans="1:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A110" s="69"/>
+      <c r="A110" s="96"/>
       <c r="B110" s="40" t="s">
         <v>6</v>
       </c>
@@ -5180,7 +5186,7 @@
       </c>
     </row>
     <row r="111" spans="1:16" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A111" s="67" t="s">
+      <c r="A111" s="94" t="s">
         <v>48</v>
       </c>
       <c r="B111" s="38" t="s">
@@ -5192,14 +5198,14 @@
       </c>
       <c r="D111" s="44">
         <f t="shared" ref="D111:D117" si="14">SUM(E111:M111)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E111" s="56"/>
       <c r="F111" s="57"/>
       <c r="G111" s="57"/>
       <c r="H111" s="57"/>
       <c r="I111" s="57">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J111" s="57"/>
       <c r="K111" s="57"/>
@@ -5214,7 +5220,7 @@
       </c>
     </row>
     <row r="112" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A112" s="68"/>
+      <c r="A112" s="95"/>
       <c r="B112" s="38" t="s">
         <v>1</v>
       </c>
@@ -5246,7 +5252,7 @@
       </c>
     </row>
     <row r="113" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A113" s="68"/>
+      <c r="A113" s="95"/>
       <c r="B113" s="38" t="s">
         <v>2</v>
       </c>
@@ -5276,7 +5282,7 @@
       </c>
     </row>
     <row r="114" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A114" s="68"/>
+      <c r="A114" s="95"/>
       <c r="B114" s="38" t="s">
         <v>3</v>
       </c>
@@ -5308,7 +5314,7 @@
       </c>
     </row>
     <row r="115" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A115" s="68"/>
+      <c r="A115" s="95"/>
       <c r="B115" s="38" t="s">
         <v>4</v>
       </c>
@@ -5318,14 +5324,14 @@
       </c>
       <c r="D115" s="44">
         <f t="shared" si="14"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E115" s="50"/>
       <c r="F115" s="51"/>
       <c r="G115" s="51"/>
       <c r="H115" s="51"/>
       <c r="I115" s="51">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J115" s="51"/>
       <c r="K115" s="51"/>
@@ -5340,7 +5346,7 @@
       </c>
     </row>
     <row r="116" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A116" s="68"/>
+      <c r="A116" s="95"/>
       <c r="B116" s="38" t="s">
         <v>5</v>
       </c>
@@ -5350,14 +5356,14 @@
       </c>
       <c r="D116" s="44">
         <f t="shared" si="14"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E116" s="50"/>
       <c r="F116" s="51"/>
       <c r="G116" s="51"/>
       <c r="H116" s="51"/>
       <c r="I116" s="51">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J116" s="51"/>
       <c r="K116" s="51"/>
@@ -5372,7 +5378,7 @@
       </c>
     </row>
     <row r="117" spans="1:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A117" s="69"/>
+      <c r="A117" s="96"/>
       <c r="B117" s="40" t="s">
         <v>6</v>
       </c>
@@ -5404,7 +5410,7 @@
       </c>
     </row>
     <row r="118" spans="1:16" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A118" s="67" t="s">
+      <c r="A118" s="94" t="s">
         <v>49</v>
       </c>
       <c r="B118" s="38" t="s">
@@ -5422,10 +5428,10 @@
       <c r="F118" s="57"/>
       <c r="G118" s="57"/>
       <c r="H118" s="57"/>
-      <c r="I118" s="57">
+      <c r="I118" s="57"/>
+      <c r="J118" s="57">
         <v>2</v>
       </c>
-      <c r="J118" s="57"/>
       <c r="K118" s="57"/>
       <c r="L118" s="57"/>
       <c r="M118" s="57"/>
@@ -5438,7 +5444,7 @@
       </c>
     </row>
     <row r="119" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A119" s="68"/>
+      <c r="A119" s="95"/>
       <c r="B119" s="38" t="s">
         <v>1</v>
       </c>
@@ -5448,16 +5454,16 @@
       </c>
       <c r="D119" s="44">
         <f t="shared" si="16"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E119" s="50"/>
       <c r="F119" s="51"/>
       <c r="G119" s="51"/>
       <c r="H119" s="51"/>
-      <c r="I119" s="51">
-        <v>1</v>
-      </c>
-      <c r="J119" s="51"/>
+      <c r="I119" s="51"/>
+      <c r="J119" s="51">
+        <v>3</v>
+      </c>
       <c r="K119" s="51"/>
       <c r="L119" s="51"/>
       <c r="M119" s="51"/>
@@ -5470,7 +5476,7 @@
       </c>
     </row>
     <row r="120" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A120" s="68"/>
+      <c r="A120" s="95"/>
       <c r="B120" s="38" t="s">
         <v>2</v>
       </c>
@@ -5480,16 +5486,16 @@
       </c>
       <c r="D120" s="44">
         <f t="shared" si="16"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E120" s="50"/>
       <c r="F120" s="51"/>
       <c r="G120" s="51"/>
       <c r="H120" s="51"/>
-      <c r="I120" s="51">
-        <v>3</v>
-      </c>
-      <c r="J120" s="51"/>
+      <c r="I120" s="51"/>
+      <c r="J120" s="51">
+        <v>2</v>
+      </c>
       <c r="K120" s="51"/>
       <c r="L120" s="51"/>
       <c r="M120" s="51"/>
@@ -5502,7 +5508,7 @@
       </c>
     </row>
     <row r="121" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A121" s="68"/>
+      <c r="A121" s="95"/>
       <c r="B121" s="38" t="s">
         <v>3</v>
       </c>
@@ -5512,16 +5518,16 @@
       </c>
       <c r="D121" s="44">
         <f t="shared" si="16"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E121" s="50"/>
       <c r="F121" s="51"/>
       <c r="G121" s="51"/>
       <c r="H121" s="51"/>
-      <c r="I121" s="51">
-        <v>1</v>
-      </c>
-      <c r="J121" s="51"/>
+      <c r="I121" s="51"/>
+      <c r="J121" s="51">
+        <v>3</v>
+      </c>
       <c r="K121" s="51"/>
       <c r="L121" s="51"/>
       <c r="M121" s="51"/>
@@ -5534,7 +5540,7 @@
       </c>
     </row>
     <row r="122" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A122" s="68"/>
+      <c r="A122" s="95"/>
       <c r="B122" s="38" t="s">
         <v>4</v>
       </c>
@@ -5544,16 +5550,16 @@
       </c>
       <c r="D122" s="44">
         <f t="shared" si="16"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E122" s="50"/>
       <c r="F122" s="51"/>
       <c r="G122" s="51"/>
       <c r="H122" s="51"/>
-      <c r="I122" s="51">
-        <v>3</v>
-      </c>
-      <c r="J122" s="51"/>
+      <c r="I122" s="51"/>
+      <c r="J122" s="51">
+        <v>4</v>
+      </c>
       <c r="K122" s="51"/>
       <c r="L122" s="51"/>
       <c r="M122" s="51"/>
@@ -5566,7 +5572,7 @@
       </c>
     </row>
     <row r="123" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A123" s="68"/>
+      <c r="A123" s="95"/>
       <c r="B123" s="38" t="s">
         <v>5</v>
       </c>
@@ -5576,16 +5582,16 @@
       </c>
       <c r="D123" s="44">
         <f t="shared" si="16"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E123" s="50"/>
       <c r="F123" s="51"/>
       <c r="G123" s="51"/>
       <c r="H123" s="51"/>
-      <c r="I123" s="51">
-        <v>4</v>
-      </c>
-      <c r="J123" s="51"/>
+      <c r="I123" s="51"/>
+      <c r="J123" s="51">
+        <v>5</v>
+      </c>
       <c r="K123" s="51"/>
       <c r="L123" s="51"/>
       <c r="M123" s="51"/>
@@ -5598,7 +5604,7 @@
       </c>
     </row>
     <row r="124" spans="1:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A124" s="69"/>
+      <c r="A124" s="96"/>
       <c r="B124" s="40" t="s">
         <v>6</v>
       </c>
@@ -5608,16 +5614,16 @@
       </c>
       <c r="D124" s="44">
         <f t="shared" si="16"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E124" s="58"/>
       <c r="F124" s="59"/>
       <c r="G124" s="59"/>
       <c r="H124" s="59"/>
-      <c r="I124" s="59">
-        <v>4</v>
-      </c>
-      <c r="J124" s="59"/>
+      <c r="I124" s="59"/>
+      <c r="J124" s="59">
+        <v>5</v>
+      </c>
       <c r="K124" s="59"/>
       <c r="L124" s="59"/>
       <c r="M124" s="59"/>
@@ -5630,7 +5636,7 @@
       </c>
     </row>
     <row r="125" spans="1:16" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A125" s="67" t="s">
+      <c r="A125" s="94" t="s">
         <v>50</v>
       </c>
       <c r="B125" s="38" t="s">
@@ -5642,16 +5648,16 @@
       </c>
       <c r="D125" s="44">
         <f t="shared" ref="D125:D138" si="18">SUM(E125:M125)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E125" s="56"/>
       <c r="F125" s="57"/>
       <c r="G125" s="57"/>
       <c r="H125" s="57"/>
-      <c r="I125" s="57">
-        <v>2</v>
-      </c>
-      <c r="J125" s="57"/>
+      <c r="I125" s="57"/>
+      <c r="J125" s="57">
+        <v>1</v>
+      </c>
       <c r="K125" s="57"/>
       <c r="L125" s="57"/>
       <c r="M125" s="57"/>
@@ -5664,7 +5670,7 @@
       </c>
     </row>
     <row r="126" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A126" s="68"/>
+      <c r="A126" s="95"/>
       <c r="B126" s="38" t="s">
         <v>1</v>
       </c>
@@ -5674,7 +5680,7 @@
       </c>
       <c r="D126" s="44">
         <f t="shared" si="18"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E126" s="50"/>
       <c r="F126" s="51"/>
@@ -5682,7 +5688,7 @@
       <c r="H126" s="51"/>
       <c r="I126" s="51"/>
       <c r="J126" s="51">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K126" s="51"/>
       <c r="L126" s="51"/>
@@ -5696,7 +5702,7 @@
       </c>
     </row>
     <row r="127" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A127" s="68"/>
+      <c r="A127" s="95"/>
       <c r="B127" s="38" t="s">
         <v>2</v>
       </c>
@@ -5706,7 +5712,7 @@
       </c>
       <c r="D127" s="44">
         <f t="shared" si="18"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E127" s="50"/>
       <c r="F127" s="51"/>
@@ -5714,7 +5720,7 @@
       <c r="H127" s="51"/>
       <c r="I127" s="51"/>
       <c r="J127" s="51">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K127" s="51"/>
       <c r="L127" s="51"/>
@@ -5728,7 +5734,7 @@
       </c>
     </row>
     <row r="128" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A128" s="68"/>
+      <c r="A128" s="95"/>
       <c r="B128" s="38" t="s">
         <v>3</v>
       </c>
@@ -5738,7 +5744,7 @@
       </c>
       <c r="D128" s="44">
         <f t="shared" si="18"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E128" s="50"/>
       <c r="F128" s="51"/>
@@ -5746,7 +5752,7 @@
       <c r="H128" s="51"/>
       <c r="I128" s="51"/>
       <c r="J128" s="51">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K128" s="51"/>
       <c r="L128" s="51"/>
@@ -5760,7 +5766,7 @@
       </c>
     </row>
     <row r="129" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A129" s="68"/>
+      <c r="A129" s="95"/>
       <c r="B129" s="38" t="s">
         <v>4</v>
       </c>
@@ -5770,7 +5776,7 @@
       </c>
       <c r="D129" s="44">
         <f t="shared" si="18"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E129" s="50"/>
       <c r="F129" s="51"/>
@@ -5778,7 +5784,7 @@
       <c r="H129" s="51"/>
       <c r="I129" s="51"/>
       <c r="J129" s="51">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="K129" s="51"/>
       <c r="L129" s="51"/>
@@ -5792,7 +5798,7 @@
       </c>
     </row>
     <row r="130" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A130" s="68"/>
+      <c r="A130" s="95"/>
       <c r="B130" s="38" t="s">
         <v>5</v>
       </c>
@@ -5802,7 +5808,7 @@
       </c>
       <c r="D130" s="44">
         <f t="shared" si="18"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E130" s="50"/>
       <c r="F130" s="51"/>
@@ -5810,7 +5816,7 @@
       <c r="H130" s="51"/>
       <c r="I130" s="51"/>
       <c r="J130" s="51">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K130" s="51"/>
       <c r="L130" s="51"/>
@@ -5824,7 +5830,7 @@
       </c>
     </row>
     <row r="131" spans="1:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A131" s="69"/>
+      <c r="A131" s="96"/>
       <c r="B131" s="40" t="s">
         <v>6</v>
       </c>
@@ -5834,7 +5840,7 @@
       </c>
       <c r="D131" s="44">
         <f t="shared" si="18"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E131" s="58"/>
       <c r="F131" s="59"/>
@@ -5842,7 +5848,7 @@
       <c r="H131" s="59"/>
       <c r="I131" s="59"/>
       <c r="J131" s="59">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K131" s="59"/>
       <c r="L131" s="59"/>
@@ -5856,7 +5862,7 @@
       </c>
     </row>
     <row r="132" spans="1:16" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A132" s="67" t="s">
+      <c r="A132" s="94" t="s">
         <v>56</v>
       </c>
       <c r="B132" s="38" t="s">
@@ -5868,7 +5874,7 @@
       </c>
       <c r="D132" s="44">
         <f t="shared" si="18"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E132" s="56"/>
       <c r="F132" s="57"/>
@@ -5876,7 +5882,7 @@
       <c r="H132" s="57"/>
       <c r="I132" s="57"/>
       <c r="J132" s="57">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K132" s="57"/>
       <c r="L132" s="57"/>
@@ -5890,7 +5896,7 @@
       </c>
     </row>
     <row r="133" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A133" s="68"/>
+      <c r="A133" s="95"/>
       <c r="B133" s="38" t="s">
         <v>1</v>
       </c>
@@ -5900,7 +5906,7 @@
       </c>
       <c r="D133" s="44">
         <f t="shared" si="18"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E133" s="50"/>
       <c r="F133" s="51"/>
@@ -5908,9 +5914,11 @@
       <c r="H133" s="51"/>
       <c r="I133" s="51"/>
       <c r="J133" s="51">
+        <v>2</v>
+      </c>
+      <c r="K133" s="51">
         <v>1</v>
       </c>
-      <c r="K133" s="51"/>
       <c r="L133" s="51"/>
       <c r="M133" s="51"/>
       <c r="N133" s="49"/>
@@ -5922,7 +5930,7 @@
       </c>
     </row>
     <row r="134" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A134" s="68"/>
+      <c r="A134" s="95"/>
       <c r="B134" s="38" t="s">
         <v>2</v>
       </c>
@@ -5932,17 +5940,17 @@
       </c>
       <c r="D134" s="44">
         <f t="shared" si="18"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E134" s="50"/>
       <c r="F134" s="51"/>
       <c r="G134" s="51"/>
       <c r="H134" s="51"/>
       <c r="I134" s="51"/>
-      <c r="J134" s="51">
-        <v>3</v>
-      </c>
-      <c r="K134" s="51"/>
+      <c r="J134" s="51"/>
+      <c r="K134" s="51">
+        <v>1</v>
+      </c>
       <c r="L134" s="51"/>
       <c r="M134" s="51"/>
       <c r="N134" s="49"/>
@@ -5954,7 +5962,7 @@
       </c>
     </row>
     <row r="135" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A135" s="68"/>
+      <c r="A135" s="95"/>
       <c r="B135" s="38" t="s">
         <v>3</v>
       </c>
@@ -5964,17 +5972,17 @@
       </c>
       <c r="D135" s="44">
         <f t="shared" si="18"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E135" s="50"/>
       <c r="F135" s="51"/>
       <c r="G135" s="51"/>
       <c r="H135" s="51"/>
       <c r="I135" s="51"/>
-      <c r="J135" s="51">
-        <v>1</v>
-      </c>
-      <c r="K135" s="51"/>
+      <c r="J135" s="51"/>
+      <c r="K135" s="51">
+        <v>3</v>
+      </c>
       <c r="L135" s="51"/>
       <c r="M135" s="51"/>
       <c r="N135" s="49"/>
@@ -5986,7 +5994,7 @@
       </c>
     </row>
     <row r="136" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A136" s="68"/>
+      <c r="A136" s="95"/>
       <c r="B136" s="38" t="s">
         <v>4</v>
       </c>
@@ -5996,17 +6004,17 @@
       </c>
       <c r="D136" s="44">
         <f t="shared" si="18"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E136" s="50"/>
       <c r="F136" s="51"/>
       <c r="G136" s="51"/>
       <c r="H136" s="51"/>
       <c r="I136" s="51"/>
-      <c r="J136" s="51">
-        <v>3</v>
-      </c>
-      <c r="K136" s="51"/>
+      <c r="J136" s="51"/>
+      <c r="K136" s="51">
+        <v>4</v>
+      </c>
       <c r="L136" s="51"/>
       <c r="M136" s="51"/>
       <c r="N136" s="49"/>
@@ -6018,7 +6026,7 @@
       </c>
     </row>
     <row r="137" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A137" s="68"/>
+      <c r="A137" s="95"/>
       <c r="B137" s="38" t="s">
         <v>5</v>
       </c>
@@ -6028,17 +6036,17 @@
       </c>
       <c r="D137" s="44">
         <f t="shared" si="18"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E137" s="50"/>
       <c r="F137" s="51"/>
       <c r="G137" s="51"/>
       <c r="H137" s="51"/>
       <c r="I137" s="51"/>
-      <c r="J137" s="51">
-        <v>4</v>
-      </c>
-      <c r="K137" s="51"/>
+      <c r="J137" s="51"/>
+      <c r="K137" s="51">
+        <v>5</v>
+      </c>
       <c r="L137" s="51"/>
       <c r="M137" s="51"/>
       <c r="N137" s="49"/>
@@ -6050,7 +6058,7 @@
       </c>
     </row>
     <row r="138" spans="1:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A138" s="69"/>
+      <c r="A138" s="96"/>
       <c r="B138" s="40" t="s">
         <v>6</v>
       </c>
@@ -6060,17 +6068,17 @@
       </c>
       <c r="D138" s="44">
         <f t="shared" si="18"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E138" s="58"/>
       <c r="F138" s="59"/>
       <c r="G138" s="59"/>
       <c r="H138" s="59"/>
       <c r="I138" s="59"/>
-      <c r="J138" s="59">
-        <v>4</v>
-      </c>
-      <c r="K138" s="59"/>
+      <c r="J138" s="59"/>
+      <c r="K138" s="59">
+        <v>5</v>
+      </c>
       <c r="L138" s="59"/>
       <c r="M138" s="59"/>
       <c r="N138" s="49"/>
@@ -6082,7 +6090,7 @@
       </c>
     </row>
     <row r="139" spans="1:16" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A139" s="67" t="s">
+      <c r="A139" s="94" t="s">
         <v>57</v>
       </c>
       <c r="B139" s="38" t="s">
@@ -6094,17 +6102,17 @@
       </c>
       <c r="D139" s="44">
         <f t="shared" ref="D139:D145" si="20">SUM(E139:M139)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E139" s="56"/>
       <c r="F139" s="57"/>
       <c r="G139" s="57"/>
       <c r="H139" s="57"/>
       <c r="I139" s="57"/>
-      <c r="J139" s="57">
-        <v>2</v>
-      </c>
-      <c r="K139" s="57"/>
+      <c r="J139" s="57"/>
+      <c r="K139" s="57">
+        <v>1</v>
+      </c>
       <c r="L139" s="57"/>
       <c r="M139" s="57"/>
       <c r="N139" s="49"/>
@@ -6116,7 +6124,7 @@
       </c>
     </row>
     <row r="140" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A140" s="68"/>
+      <c r="A140" s="95"/>
       <c r="B140" s="38" t="s">
         <v>1</v>
       </c>
@@ -6126,17 +6134,17 @@
       </c>
       <c r="D140" s="44">
         <f t="shared" si="20"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E140" s="50"/>
       <c r="F140" s="51"/>
       <c r="G140" s="51"/>
       <c r="H140" s="51"/>
       <c r="I140" s="51"/>
-      <c r="J140" s="51">
-        <v>1</v>
-      </c>
-      <c r="K140" s="51"/>
+      <c r="J140" s="51"/>
+      <c r="K140" s="51">
+        <v>3</v>
+      </c>
       <c r="L140" s="51"/>
       <c r="M140" s="51"/>
       <c r="N140" s="49"/>
@@ -6148,7 +6156,7 @@
       </c>
     </row>
     <row r="141" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A141" s="68"/>
+      <c r="A141" s="95"/>
       <c r="B141" s="38" t="s">
         <v>2</v>
       </c>
@@ -6158,17 +6166,17 @@
       </c>
       <c r="D141" s="44">
         <f t="shared" si="20"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E141" s="50"/>
       <c r="F141" s="51"/>
       <c r="G141" s="51"/>
       <c r="H141" s="51"/>
       <c r="I141" s="51"/>
-      <c r="J141" s="51">
-        <v>3</v>
-      </c>
-      <c r="K141" s="51"/>
+      <c r="J141" s="51"/>
+      <c r="K141" s="51">
+        <v>1</v>
+      </c>
       <c r="L141" s="51"/>
       <c r="M141" s="51"/>
       <c r="N141" s="49"/>
@@ -6180,7 +6188,7 @@
       </c>
     </row>
     <row r="142" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A142" s="68"/>
+      <c r="A142" s="95"/>
       <c r="B142" s="38" t="s">
         <v>3</v>
       </c>
@@ -6190,17 +6198,17 @@
       </c>
       <c r="D142" s="44">
         <f t="shared" si="20"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E142" s="50"/>
       <c r="F142" s="51"/>
       <c r="G142" s="51"/>
       <c r="H142" s="51"/>
       <c r="I142" s="51"/>
-      <c r="J142" s="51">
-        <v>1</v>
-      </c>
-      <c r="K142" s="51"/>
+      <c r="J142" s="51"/>
+      <c r="K142" s="51">
+        <v>3</v>
+      </c>
       <c r="L142" s="51"/>
       <c r="M142" s="51"/>
       <c r="N142" s="49"/>
@@ -6212,7 +6220,7 @@
       </c>
     </row>
     <row r="143" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A143" s="68"/>
+      <c r="A143" s="95"/>
       <c r="B143" s="38" t="s">
         <v>4</v>
       </c>
@@ -6222,17 +6230,17 @@
       </c>
       <c r="D143" s="44">
         <f t="shared" si="20"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E143" s="50"/>
       <c r="F143" s="51"/>
       <c r="G143" s="51"/>
       <c r="H143" s="51"/>
       <c r="I143" s="51"/>
-      <c r="J143" s="51">
-        <v>3</v>
-      </c>
-      <c r="K143" s="51"/>
+      <c r="J143" s="51"/>
+      <c r="K143" s="51">
+        <v>5</v>
+      </c>
       <c r="L143" s="51"/>
       <c r="M143" s="51"/>
       <c r="N143" s="49"/>
@@ -6244,7 +6252,7 @@
       </c>
     </row>
     <row r="144" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A144" s="68"/>
+      <c r="A144" s="95"/>
       <c r="B144" s="38" t="s">
         <v>5</v>
       </c>
@@ -6254,17 +6262,17 @@
       </c>
       <c r="D144" s="44">
         <f t="shared" si="20"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E144" s="50"/>
       <c r="F144" s="51"/>
       <c r="G144" s="51"/>
       <c r="H144" s="51"/>
       <c r="I144" s="51"/>
-      <c r="J144" s="51">
-        <v>4</v>
-      </c>
-      <c r="K144" s="51"/>
+      <c r="J144" s="51"/>
+      <c r="K144" s="51">
+        <v>5</v>
+      </c>
       <c r="L144" s="51"/>
       <c r="M144" s="51"/>
       <c r="N144" s="49"/>
@@ -6276,7 +6284,7 @@
       </c>
     </row>
     <row r="145" spans="1:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A145" s="69"/>
+      <c r="A145" s="96"/>
       <c r="B145" s="40" t="s">
         <v>6</v>
       </c>
@@ -6286,18 +6294,16 @@
       </c>
       <c r="D145" s="44">
         <f t="shared" si="20"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E145" s="58"/>
       <c r="F145" s="59"/>
       <c r="G145" s="59"/>
       <c r="H145" s="59"/>
       <c r="I145" s="59"/>
-      <c r="J145" s="59">
-        <v>2</v>
-      </c>
+      <c r="J145" s="59"/>
       <c r="K145" s="59">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="L145" s="59"/>
       <c r="M145" s="59"/>
@@ -6310,7 +6316,7 @@
       </c>
     </row>
     <row r="146" spans="1:16" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A146" s="67" t="s">
+      <c r="A146" s="94" t="s">
         <v>51</v>
       </c>
       <c r="B146" s="38" t="s">
@@ -6322,7 +6328,7 @@
       </c>
       <c r="D146" s="44">
         <f t="shared" ref="D146:D152" si="22">SUM(E146:M146)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E146" s="56"/>
       <c r="F146" s="57"/>
@@ -6331,7 +6337,7 @@
       <c r="I146" s="57"/>
       <c r="J146" s="57"/>
       <c r="K146" s="57">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L146" s="57"/>
       <c r="M146" s="57"/>
@@ -6344,7 +6350,7 @@
       </c>
     </row>
     <row r="147" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A147" s="68"/>
+      <c r="A147" s="95"/>
       <c r="B147" s="38" t="s">
         <v>1</v>
       </c>
@@ -6354,7 +6360,7 @@
       </c>
       <c r="D147" s="44">
         <f t="shared" si="22"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E147" s="50"/>
       <c r="F147" s="51"/>
@@ -6363,7 +6369,7 @@
       <c r="I147" s="51"/>
       <c r="J147" s="51"/>
       <c r="K147" s="51">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L147" s="51"/>
       <c r="M147" s="51"/>
@@ -6376,7 +6382,7 @@
       </c>
     </row>
     <row r="148" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A148" s="68"/>
+      <c r="A148" s="95"/>
       <c r="B148" s="38" t="s">
         <v>2</v>
       </c>
@@ -6386,7 +6392,7 @@
       </c>
       <c r="D148" s="44">
         <f t="shared" si="22"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E148" s="50"/>
       <c r="F148" s="51"/>
@@ -6395,7 +6401,7 @@
       <c r="I148" s="51"/>
       <c r="J148" s="51"/>
       <c r="K148" s="51">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L148" s="51"/>
       <c r="M148" s="51"/>
@@ -6408,7 +6414,7 @@
       </c>
     </row>
     <row r="149" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A149" s="68"/>
+      <c r="A149" s="95"/>
       <c r="B149" s="38" t="s">
         <v>3</v>
       </c>
@@ -6418,7 +6424,7 @@
       </c>
       <c r="D149" s="44">
         <f t="shared" si="22"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E149" s="50"/>
       <c r="F149" s="51"/>
@@ -6427,7 +6433,7 @@
       <c r="I149" s="51"/>
       <c r="J149" s="51"/>
       <c r="K149" s="51">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L149" s="51"/>
       <c r="M149" s="51"/>
@@ -6440,7 +6446,7 @@
       </c>
     </row>
     <row r="150" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A150" s="68"/>
+      <c r="A150" s="95"/>
       <c r="B150" s="38" t="s">
         <v>4</v>
       </c>
@@ -6450,7 +6456,7 @@
       </c>
       <c r="D150" s="44">
         <f t="shared" si="22"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E150" s="50"/>
       <c r="F150" s="51"/>
@@ -6458,10 +6464,10 @@
       <c r="H150" s="51"/>
       <c r="I150" s="51"/>
       <c r="J150" s="51"/>
-      <c r="K150" s="51">
-        <v>3</v>
-      </c>
-      <c r="L150" s="51"/>
+      <c r="K150" s="51"/>
+      <c r="L150" s="51">
+        <v>5</v>
+      </c>
       <c r="M150" s="51"/>
       <c r="N150" s="49"/>
       <c r="O150">
@@ -6472,7 +6478,7 @@
       </c>
     </row>
     <row r="151" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A151" s="68"/>
+      <c r="A151" s="95"/>
       <c r="B151" s="38" t="s">
         <v>5</v>
       </c>
@@ -6482,7 +6488,7 @@
       </c>
       <c r="D151" s="44">
         <f t="shared" si="22"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E151" s="50"/>
       <c r="F151" s="51"/>
@@ -6490,10 +6496,10 @@
       <c r="H151" s="51"/>
       <c r="I151" s="51"/>
       <c r="J151" s="51"/>
-      <c r="K151" s="51">
-        <v>4</v>
-      </c>
-      <c r="L151" s="51"/>
+      <c r="K151" s="51"/>
+      <c r="L151" s="51">
+        <v>5</v>
+      </c>
       <c r="M151" s="51"/>
       <c r="N151" s="49"/>
       <c r="O151">
@@ -6504,7 +6510,7 @@
       </c>
     </row>
     <row r="152" spans="1:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A152" s="69"/>
+      <c r="A152" s="96"/>
       <c r="B152" s="40" t="s">
         <v>6</v>
       </c>
@@ -6514,7 +6520,7 @@
       </c>
       <c r="D152" s="44">
         <f t="shared" si="22"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E152" s="58"/>
       <c r="F152" s="59"/>
@@ -6522,10 +6528,10 @@
       <c r="H152" s="59"/>
       <c r="I152" s="59"/>
       <c r="J152" s="59"/>
-      <c r="K152" s="59">
-        <v>4</v>
-      </c>
-      <c r="L152" s="59"/>
+      <c r="K152" s="59"/>
+      <c r="L152" s="59">
+        <v>5</v>
+      </c>
       <c r="M152" s="59"/>
       <c r="N152" s="49"/>
       <c r="O152">
@@ -6536,7 +6542,7 @@
       </c>
     </row>
     <row r="153" spans="1:16" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A153" s="67" t="s">
+      <c r="A153" s="94" t="s">
         <v>52</v>
       </c>
       <c r="B153" s="38" t="s">
@@ -6548,7 +6554,7 @@
       </c>
       <c r="D153" s="44">
         <f t="shared" ref="D153:D159" si="24">SUM(E153:M153)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E153" s="56"/>
       <c r="F153" s="57"/>
@@ -6556,10 +6562,10 @@
       <c r="H153" s="57"/>
       <c r="I153" s="57"/>
       <c r="J153" s="57"/>
-      <c r="K153" s="57">
-        <v>2</v>
-      </c>
-      <c r="L153" s="57"/>
+      <c r="K153" s="57"/>
+      <c r="L153" s="57">
+        <v>1</v>
+      </c>
       <c r="M153" s="57"/>
       <c r="N153" s="49"/>
       <c r="O153">
@@ -6570,7 +6576,7 @@
       </c>
     </row>
     <row r="154" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A154" s="68"/>
+      <c r="A154" s="95"/>
       <c r="B154" s="38" t="s">
         <v>1</v>
       </c>
@@ -6580,7 +6586,7 @@
       </c>
       <c r="D154" s="44">
         <f t="shared" si="24"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E154" s="50"/>
       <c r="F154" s="51"/>
@@ -6589,7 +6595,9 @@
       <c r="I154" s="51"/>
       <c r="J154" s="51"/>
       <c r="K154" s="51"/>
-      <c r="L154" s="51"/>
+      <c r="L154" s="51">
+        <v>3</v>
+      </c>
       <c r="M154" s="51"/>
       <c r="N154" s="49"/>
       <c r="O154">
@@ -6600,7 +6608,7 @@
       </c>
     </row>
     <row r="155" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A155" s="68"/>
+      <c r="A155" s="95"/>
       <c r="B155" s="38" t="s">
         <v>2</v>
       </c>
@@ -6610,7 +6618,7 @@
       </c>
       <c r="D155" s="44">
         <f t="shared" si="24"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E155" s="50"/>
       <c r="F155" s="51"/>
@@ -6618,10 +6626,10 @@
       <c r="H155" s="51"/>
       <c r="I155" s="51"/>
       <c r="J155" s="51"/>
-      <c r="K155" s="51">
-        <v>3</v>
-      </c>
-      <c r="L155" s="51"/>
+      <c r="K155" s="51"/>
+      <c r="L155" s="51">
+        <v>1</v>
+      </c>
       <c r="M155" s="51"/>
       <c r="N155" s="49"/>
       <c r="O155">
@@ -6632,7 +6640,7 @@
       </c>
     </row>
     <row r="156" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A156" s="68"/>
+      <c r="A156" s="95"/>
       <c r="B156" s="38" t="s">
         <v>3</v>
       </c>
@@ -6642,7 +6650,7 @@
       </c>
       <c r="D156" s="44">
         <f t="shared" si="24"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E156" s="50"/>
       <c r="F156" s="51"/>
@@ -6651,7 +6659,9 @@
       <c r="I156" s="51"/>
       <c r="J156" s="51"/>
       <c r="K156" s="51"/>
-      <c r="L156" s="51"/>
+      <c r="L156" s="51">
+        <v>3</v>
+      </c>
       <c r="M156" s="51"/>
       <c r="N156" s="49"/>
       <c r="O156">
@@ -6662,7 +6672,7 @@
       </c>
     </row>
     <row r="157" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A157" s="68"/>
+      <c r="A157" s="95"/>
       <c r="B157" s="38" t="s">
         <v>4</v>
       </c>
@@ -6672,7 +6682,7 @@
       </c>
       <c r="D157" s="44">
         <f t="shared" si="24"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E157" s="50"/>
       <c r="F157" s="51"/>
@@ -6680,10 +6690,10 @@
       <c r="H157" s="51"/>
       <c r="I157" s="51"/>
       <c r="J157" s="51"/>
-      <c r="K157" s="51">
-        <v>3</v>
-      </c>
-      <c r="L157" s="51"/>
+      <c r="K157" s="51"/>
+      <c r="L157" s="51">
+        <v>4</v>
+      </c>
       <c r="M157" s="51"/>
       <c r="N157" s="49"/>
       <c r="O157">
@@ -6694,7 +6704,7 @@
       </c>
     </row>
     <row r="158" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A158" s="68"/>
+      <c r="A158" s="95"/>
       <c r="B158" s="38" t="s">
         <v>5</v>
       </c>
@@ -6704,7 +6714,7 @@
       </c>
       <c r="D158" s="44">
         <f t="shared" si="24"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E158" s="50"/>
       <c r="F158" s="51"/>
@@ -6712,10 +6722,10 @@
       <c r="H158" s="51"/>
       <c r="I158" s="51"/>
       <c r="J158" s="51"/>
-      <c r="K158" s="51">
-        <v>4</v>
-      </c>
-      <c r="L158" s="51"/>
+      <c r="K158" s="51"/>
+      <c r="L158" s="51">
+        <v>5</v>
+      </c>
       <c r="M158" s="51"/>
       <c r="N158" s="49"/>
       <c r="O158">
@@ -6726,7 +6736,7 @@
       </c>
     </row>
     <row r="159" spans="1:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A159" s="69"/>
+      <c r="A159" s="96"/>
       <c r="B159" s="40" t="s">
         <v>6</v>
       </c>
@@ -6744,10 +6754,10 @@
       <c r="H159" s="59"/>
       <c r="I159" s="59"/>
       <c r="J159" s="59"/>
-      <c r="K159" s="59">
-        <v>5</v>
-      </c>
-      <c r="L159" s="59"/>
+      <c r="K159" s="59"/>
+      <c r="L159" s="59">
+        <v>5</v>
+      </c>
       <c r="M159" s="59"/>
       <c r="N159" s="49"/>
       <c r="O159">
@@ -6758,7 +6768,7 @@
       </c>
     </row>
     <row r="160" spans="1:16" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A160" s="67" t="s">
+      <c r="A160" s="94" t="s">
         <v>53</v>
       </c>
       <c r="B160" s="38" t="s">
@@ -6770,7 +6780,7 @@
       </c>
       <c r="D160" s="44">
         <f t="shared" ref="D160:D166" si="26">SUM(E160:M160)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E160" s="56"/>
       <c r="F160" s="57"/>
@@ -6778,10 +6788,10 @@
       <c r="H160" s="57"/>
       <c r="I160" s="57"/>
       <c r="J160" s="57"/>
-      <c r="K160" s="57">
-        <v>2</v>
-      </c>
-      <c r="L160" s="57"/>
+      <c r="K160" s="57"/>
+      <c r="L160" s="57">
+        <v>1</v>
+      </c>
       <c r="M160" s="57"/>
       <c r="N160" s="49"/>
       <c r="O160">
@@ -6792,7 +6802,7 @@
       </c>
     </row>
     <row r="161" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A161" s="68"/>
+      <c r="A161" s="95"/>
       <c r="B161" s="38" t="s">
         <v>1</v>
       </c>
@@ -6802,7 +6812,7 @@
       </c>
       <c r="D161" s="44">
         <f t="shared" si="26"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E161" s="50"/>
       <c r="F161" s="51"/>
@@ -6810,10 +6820,10 @@
       <c r="H161" s="51"/>
       <c r="I161" s="51"/>
       <c r="J161" s="51"/>
-      <c r="K161" s="51">
-        <v>1</v>
-      </c>
-      <c r="L161" s="51"/>
+      <c r="K161" s="51"/>
+      <c r="L161" s="51">
+        <v>3</v>
+      </c>
       <c r="M161" s="51"/>
       <c r="N161" s="49"/>
       <c r="O161">
@@ -6824,7 +6834,7 @@
       </c>
     </row>
     <row r="162" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A162" s="68"/>
+      <c r="A162" s="95"/>
       <c r="B162" s="38" t="s">
         <v>2</v>
       </c>
@@ -6834,7 +6844,7 @@
       </c>
       <c r="D162" s="44">
         <f t="shared" si="26"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E162" s="50"/>
       <c r="F162" s="51"/>
@@ -6842,10 +6852,10 @@
       <c r="H162" s="51"/>
       <c r="I162" s="51"/>
       <c r="J162" s="51"/>
-      <c r="K162" s="51">
-        <v>2</v>
-      </c>
-      <c r="L162" s="51"/>
+      <c r="K162" s="51"/>
+      <c r="L162" s="51">
+        <v>1</v>
+      </c>
       <c r="M162" s="51"/>
       <c r="N162" s="49"/>
       <c r="O162">
@@ -6856,7 +6866,7 @@
       </c>
     </row>
     <row r="163" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A163" s="68"/>
+      <c r="A163" s="95"/>
       <c r="B163" s="38" t="s">
         <v>3</v>
       </c>
@@ -6866,7 +6876,7 @@
       </c>
       <c r="D163" s="44">
         <f t="shared" si="26"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E163" s="50"/>
       <c r="F163" s="51"/>
@@ -6874,10 +6884,10 @@
       <c r="H163" s="51"/>
       <c r="I163" s="51"/>
       <c r="J163" s="51"/>
-      <c r="K163" s="51">
-        <v>1</v>
-      </c>
-      <c r="L163" s="51"/>
+      <c r="K163" s="51"/>
+      <c r="L163" s="51">
+        <v>3</v>
+      </c>
       <c r="M163" s="51"/>
       <c r="N163" s="49"/>
       <c r="O163">
@@ -6888,7 +6898,7 @@
       </c>
     </row>
     <row r="164" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A164" s="68"/>
+      <c r="A164" s="95"/>
       <c r="B164" s="38" t="s">
         <v>4</v>
       </c>
@@ -6898,7 +6908,7 @@
       </c>
       <c r="D164" s="44">
         <f t="shared" si="26"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E164" s="50"/>
       <c r="F164" s="51"/>
@@ -6906,10 +6916,10 @@
       <c r="H164" s="51"/>
       <c r="I164" s="51"/>
       <c r="J164" s="51"/>
-      <c r="K164" s="51">
-        <v>3</v>
-      </c>
-      <c r="L164" s="51"/>
+      <c r="K164" s="51"/>
+      <c r="L164" s="51">
+        <v>5</v>
+      </c>
       <c r="M164" s="51"/>
       <c r="N164" s="49"/>
       <c r="O164">
@@ -6920,7 +6930,7 @@
       </c>
     </row>
     <row r="165" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A165" s="68"/>
+      <c r="A165" s="95"/>
       <c r="B165" s="38" t="s">
         <v>5</v>
       </c>
@@ -6930,7 +6940,7 @@
       </c>
       <c r="D165" s="44">
         <f t="shared" si="26"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E165" s="50"/>
       <c r="F165" s="51"/>
@@ -6938,11 +6948,11 @@
       <c r="H165" s="51"/>
       <c r="I165" s="51"/>
       <c r="J165" s="51"/>
-      <c r="K165" s="51">
-        <v>4</v>
-      </c>
+      <c r="K165" s="51"/>
       <c r="L165" s="51"/>
-      <c r="M165" s="51"/>
+      <c r="M165" s="51">
+        <v>5</v>
+      </c>
       <c r="N165" s="49"/>
       <c r="O165">
         <v>26</v>
@@ -6952,7 +6962,7 @@
       </c>
     </row>
     <row r="166" spans="1:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A166" s="69"/>
+      <c r="A166" s="96"/>
       <c r="B166" s="40" t="s">
         <v>6</v>
       </c>
@@ -6962,7 +6972,7 @@
       </c>
       <c r="D166" s="44">
         <f t="shared" si="26"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E166" s="58"/>
       <c r="F166" s="59"/>
@@ -6971,10 +6981,10 @@
       <c r="I166" s="59"/>
       <c r="J166" s="59"/>
       <c r="K166" s="59"/>
-      <c r="L166" s="59">
-        <v>4</v>
-      </c>
-      <c r="M166" s="59"/>
+      <c r="L166" s="59"/>
+      <c r="M166" s="59">
+        <v>5</v>
+      </c>
       <c r="N166" s="49"/>
       <c r="O166">
         <v>27</v>
@@ -6984,7 +6994,7 @@
       </c>
     </row>
     <row r="167" spans="1:16" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A167" s="67" t="s">
+      <c r="A167" s="94" t="s">
         <v>58</v>
       </c>
       <c r="B167" s="38" t="s">
@@ -6996,7 +7006,7 @@
       </c>
       <c r="D167" s="44">
         <f t="shared" ref="D167:D180" si="28">SUM(E167:M167)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E167" s="56"/>
       <c r="F167" s="57"/>
@@ -7005,10 +7015,10 @@
       <c r="I167" s="57"/>
       <c r="J167" s="57"/>
       <c r="K167" s="57"/>
-      <c r="L167" s="57">
-        <v>2</v>
-      </c>
-      <c r="M167" s="57"/>
+      <c r="L167" s="57"/>
+      <c r="M167" s="57">
+        <v>1</v>
+      </c>
       <c r="N167" s="49"/>
       <c r="O167">
         <v>28</v>
@@ -7018,7 +7028,7 @@
       </c>
     </row>
     <row r="168" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A168" s="68"/>
+      <c r="A168" s="95"/>
       <c r="B168" s="38" t="s">
         <v>1</v>
       </c>
@@ -7028,7 +7038,7 @@
       </c>
       <c r="D168" s="44">
         <f t="shared" si="28"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E168" s="50"/>
       <c r="F168" s="51"/>
@@ -7037,10 +7047,10 @@
       <c r="I168" s="51"/>
       <c r="J168" s="51"/>
       <c r="K168" s="51"/>
-      <c r="L168" s="51">
-        <v>1</v>
-      </c>
-      <c r="M168" s="51"/>
+      <c r="L168" s="51"/>
+      <c r="M168" s="51">
+        <v>3</v>
+      </c>
       <c r="N168" s="49"/>
       <c r="O168">
         <v>29</v>
@@ -7050,7 +7060,7 @@
       </c>
     </row>
     <row r="169" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A169" s="68"/>
+      <c r="A169" s="95"/>
       <c r="B169" s="38" t="s">
         <v>2</v>
       </c>
@@ -7060,7 +7070,7 @@
       </c>
       <c r="D169" s="44">
         <f t="shared" si="28"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E169" s="50"/>
       <c r="F169" s="51"/>
@@ -7069,10 +7079,10 @@
       <c r="I169" s="51"/>
       <c r="J169" s="51"/>
       <c r="K169" s="51"/>
-      <c r="L169" s="51">
-        <v>3</v>
-      </c>
-      <c r="M169" s="51"/>
+      <c r="L169" s="51"/>
+      <c r="M169" s="51">
+        <v>1</v>
+      </c>
       <c r="N169" s="49"/>
       <c r="O169">
         <v>30</v>
@@ -7082,7 +7092,7 @@
       </c>
     </row>
     <row r="170" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A170" s="68"/>
+      <c r="A170" s="95"/>
       <c r="B170" s="38" t="s">
         <v>3</v>
       </c>
@@ -7092,7 +7102,7 @@
       </c>
       <c r="D170" s="44">
         <f t="shared" si="28"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E170" s="50"/>
       <c r="F170" s="51"/>
@@ -7101,10 +7111,10 @@
       <c r="I170" s="51"/>
       <c r="J170" s="51"/>
       <c r="K170" s="51"/>
-      <c r="L170" s="51">
-        <v>1</v>
-      </c>
-      <c r="M170" s="51"/>
+      <c r="L170" s="51"/>
+      <c r="M170" s="51">
+        <v>3</v>
+      </c>
       <c r="N170" s="49"/>
       <c r="O170">
         <v>1</v>
@@ -7114,7 +7124,7 @@
       </c>
     </row>
     <row r="171" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A171" s="68"/>
+      <c r="A171" s="95"/>
       <c r="B171" s="38" t="s">
         <v>4</v>
       </c>
@@ -7124,7 +7134,7 @@
       </c>
       <c r="D171" s="44">
         <f t="shared" si="28"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E171" s="50"/>
       <c r="F171" s="51"/>
@@ -7133,10 +7143,10 @@
       <c r="I171" s="51"/>
       <c r="J171" s="51"/>
       <c r="K171" s="51"/>
-      <c r="L171" s="51">
-        <v>3</v>
-      </c>
-      <c r="M171" s="51"/>
+      <c r="L171" s="51"/>
+      <c r="M171" s="51">
+        <v>4</v>
+      </c>
       <c r="N171" s="49"/>
       <c r="O171">
         <v>2</v>
@@ -7146,7 +7156,7 @@
       </c>
     </row>
     <row r="172" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A172" s="68"/>
+      <c r="A172" s="95"/>
       <c r="B172" s="38" t="s">
         <v>5</v>
       </c>
@@ -7165,10 +7175,10 @@
       <c r="I172" s="51"/>
       <c r="J172" s="51"/>
       <c r="K172" s="51"/>
-      <c r="L172" s="51">
+      <c r="L172" s="51"/>
+      <c r="M172" s="51">
         <v>4</v>
       </c>
-      <c r="M172" s="51"/>
       <c r="N172" s="49"/>
       <c r="O172">
         <v>3</v>
@@ -7178,7 +7188,7 @@
       </c>
     </row>
     <row r="173" spans="1:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A173" s="69"/>
+      <c r="A173" s="96"/>
       <c r="B173" s="40" t="s">
         <v>6</v>
       </c>
@@ -7197,10 +7207,10 @@
       <c r="I173" s="59"/>
       <c r="J173" s="59"/>
       <c r="K173" s="59"/>
-      <c r="L173" s="59">
+      <c r="L173" s="59"/>
+      <c r="M173" s="59">
         <v>4</v>
       </c>
-      <c r="M173" s="59"/>
       <c r="N173" s="49"/>
       <c r="O173">
         <v>4</v>
@@ -7210,7 +7220,7 @@
       </c>
     </row>
     <row r="174" spans="1:16" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A174" s="67" t="s">
+      <c r="A174" s="94" t="s">
         <v>54</v>
       </c>
       <c r="B174" s="38" t="s">
@@ -7222,7 +7232,7 @@
       </c>
       <c r="D174" s="44">
         <f t="shared" si="28"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E174" s="56"/>
       <c r="F174" s="57"/>
@@ -7231,10 +7241,10 @@
       <c r="I174" s="57"/>
       <c r="J174" s="57"/>
       <c r="K174" s="57"/>
-      <c r="L174" s="57">
-        <v>2</v>
-      </c>
-      <c r="M174" s="57"/>
+      <c r="L174" s="57"/>
+      <c r="M174" s="57">
+        <v>1</v>
+      </c>
       <c r="N174" s="49"/>
       <c r="O174">
         <v>5</v>
@@ -7244,7 +7254,7 @@
       </c>
     </row>
     <row r="175" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A175" s="68"/>
+      <c r="A175" s="95"/>
       <c r="B175" s="38" t="s">
         <v>1</v>
       </c>
@@ -7254,7 +7264,7 @@
       </c>
       <c r="D175" s="44">
         <f t="shared" si="28"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E175" s="50"/>
       <c r="F175" s="51"/>
@@ -7263,10 +7273,10 @@
       <c r="I175" s="51"/>
       <c r="J175" s="51"/>
       <c r="K175" s="51"/>
-      <c r="L175" s="51">
-        <v>1</v>
-      </c>
-      <c r="M175" s="51"/>
+      <c r="L175" s="51"/>
+      <c r="M175" s="51">
+        <v>3</v>
+      </c>
       <c r="N175" s="49"/>
       <c r="O175">
         <v>6</v>
@@ -7276,7 +7286,7 @@
       </c>
     </row>
     <row r="176" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A176" s="68"/>
+      <c r="A176" s="95"/>
       <c r="B176" s="38" t="s">
         <v>2</v>
       </c>
@@ -7286,7 +7296,7 @@
       </c>
       <c r="D176" s="44">
         <f t="shared" si="28"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E176" s="50"/>
       <c r="F176" s="51"/>
@@ -7295,10 +7305,10 @@
       <c r="I176" s="51"/>
       <c r="J176" s="51"/>
       <c r="K176" s="51"/>
-      <c r="L176" s="51">
-        <v>3</v>
-      </c>
-      <c r="M176" s="51"/>
+      <c r="L176" s="51"/>
+      <c r="M176" s="51">
+        <v>1</v>
+      </c>
       <c r="N176" s="49"/>
       <c r="O176">
         <v>7</v>
@@ -7308,7 +7318,7 @@
       </c>
     </row>
     <row r="177" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A177" s="68"/>
+      <c r="A177" s="95"/>
       <c r="B177" s="38" t="s">
         <v>3</v>
       </c>
@@ -7327,10 +7337,10 @@
       <c r="I177" s="51"/>
       <c r="J177" s="51"/>
       <c r="K177" s="51"/>
-      <c r="L177" s="51">
+      <c r="L177" s="51"/>
+      <c r="M177" s="51">
         <v>1</v>
       </c>
-      <c r="M177" s="51"/>
       <c r="N177" s="49"/>
       <c r="O177">
         <v>8</v>
@@ -7340,7 +7350,7 @@
       </c>
     </row>
     <row r="178" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A178" s="68"/>
+      <c r="A178" s="95"/>
       <c r="B178" s="38" t="s">
         <v>4</v>
       </c>
@@ -7350,7 +7360,7 @@
       </c>
       <c r="D178" s="44">
         <f t="shared" si="28"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E178" s="50"/>
       <c r="F178" s="51"/>
@@ -7359,10 +7369,10 @@
       <c r="I178" s="51"/>
       <c r="J178" s="51"/>
       <c r="K178" s="51"/>
-      <c r="L178" s="51">
-        <v>3</v>
-      </c>
-      <c r="M178" s="51"/>
+      <c r="L178" s="51"/>
+      <c r="M178" s="51">
+        <v>4</v>
+      </c>
       <c r="N178" s="49"/>
       <c r="O178">
         <v>9</v>
@@ -7372,7 +7382,7 @@
       </c>
     </row>
     <row r="179" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A179" s="68"/>
+      <c r="A179" s="95"/>
       <c r="B179" s="38" t="s">
         <v>5</v>
       </c>
@@ -7382,7 +7392,7 @@
       </c>
       <c r="D179" s="44">
         <f t="shared" si="28"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E179" s="50"/>
       <c r="F179" s="51"/>
@@ -7391,10 +7401,10 @@
       <c r="I179" s="51"/>
       <c r="J179" s="51"/>
       <c r="K179" s="51"/>
-      <c r="L179" s="51">
-        <v>4</v>
-      </c>
-      <c r="M179" s="51"/>
+      <c r="L179" s="51"/>
+      <c r="M179" s="51">
+        <v>5</v>
+      </c>
       <c r="N179" s="49"/>
       <c r="O179">
         <v>10</v>
@@ -7404,7 +7414,7 @@
       </c>
     </row>
     <row r="180" spans="1:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A180" s="69"/>
+      <c r="A180" s="96"/>
       <c r="B180" s="40" t="s">
         <v>6</v>
       </c>
@@ -7414,7 +7424,7 @@
       </c>
       <c r="D180" s="44">
         <f t="shared" si="28"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E180" s="58"/>
       <c r="F180" s="59"/>
@@ -7423,10 +7433,10 @@
       <c r="I180" s="59"/>
       <c r="J180" s="59"/>
       <c r="K180" s="59"/>
-      <c r="L180" s="59">
-        <v>4</v>
-      </c>
-      <c r="M180" s="59"/>
+      <c r="L180" s="59"/>
+      <c r="M180" s="59">
+        <v>5</v>
+      </c>
       <c r="N180" s="49"/>
       <c r="O180">
         <v>11</v>
@@ -7436,7 +7446,7 @@
       </c>
     </row>
     <row r="181" spans="1:16" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A181" s="67" t="s">
+      <c r="A181" s="94" t="s">
         <v>55</v>
       </c>
       <c r="B181" s="38" t="s">
@@ -7448,7 +7458,7 @@
       </c>
       <c r="D181" s="44">
         <f t="shared" ref="D181:D187" si="30">SUM(E181:M181)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E181" s="56"/>
       <c r="F181" s="57"/>
@@ -7457,9 +7467,7 @@
       <c r="I181" s="57"/>
       <c r="J181" s="57"/>
       <c r="K181" s="57"/>
-      <c r="L181" s="57">
-        <v>2</v>
-      </c>
+      <c r="L181" s="57"/>
       <c r="M181" s="57"/>
       <c r="N181" s="49"/>
       <c r="O181">
@@ -7470,7 +7478,7 @@
       </c>
     </row>
     <row r="182" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A182" s="68"/>
+      <c r="A182" s="95"/>
       <c r="B182" s="38" t="s">
         <v>1</v>
       </c>
@@ -7480,7 +7488,7 @@
       </c>
       <c r="D182" s="44">
         <f t="shared" si="30"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E182" s="50"/>
       <c r="F182" s="51"/>
@@ -7489,9 +7497,7 @@
       <c r="I182" s="51"/>
       <c r="J182" s="51"/>
       <c r="K182" s="51"/>
-      <c r="L182" s="51">
-        <v>1</v>
-      </c>
+      <c r="L182" s="51"/>
       <c r="M182" s="51"/>
       <c r="N182" s="49"/>
       <c r="O182">
@@ -7502,7 +7508,7 @@
       </c>
     </row>
     <row r="183" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A183" s="68"/>
+      <c r="A183" s="95"/>
       <c r="B183" s="38" t="s">
         <v>2</v>
       </c>
@@ -7512,7 +7518,7 @@
       </c>
       <c r="D183" s="44">
         <f t="shared" si="30"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E183" s="50"/>
       <c r="F183" s="51"/>
@@ -7521,9 +7527,7 @@
       <c r="I183" s="51"/>
       <c r="J183" s="51"/>
       <c r="K183" s="51"/>
-      <c r="L183" s="51">
-        <v>3</v>
-      </c>
+      <c r="L183" s="51"/>
       <c r="M183" s="51"/>
       <c r="N183" s="49"/>
       <c r="O183">
@@ -7534,7 +7538,7 @@
       </c>
     </row>
     <row r="184" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A184" s="68"/>
+      <c r="A184" s="95"/>
       <c r="B184" s="38" t="s">
         <v>3</v>
       </c>
@@ -7544,7 +7548,7 @@
       </c>
       <c r="D184" s="44">
         <f t="shared" si="30"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E184" s="50"/>
       <c r="F184" s="51"/>
@@ -7553,9 +7557,7 @@
       <c r="I184" s="51"/>
       <c r="J184" s="51"/>
       <c r="K184" s="51"/>
-      <c r="L184" s="51">
-        <v>1</v>
-      </c>
+      <c r="L184" s="51"/>
       <c r="M184" s="51"/>
       <c r="N184" s="49"/>
       <c r="O184">
@@ -7566,7 +7568,7 @@
       </c>
     </row>
     <row r="185" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A185" s="68"/>
+      <c r="A185" s="95"/>
       <c r="B185" s="38" t="s">
         <v>4</v>
       </c>
@@ -7576,7 +7578,7 @@
       </c>
       <c r="D185" s="44">
         <f t="shared" si="30"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E185" s="50"/>
       <c r="F185" s="51"/>
@@ -7585,9 +7587,7 @@
       <c r="I185" s="51"/>
       <c r="J185" s="51"/>
       <c r="K185" s="51"/>
-      <c r="L185" s="51">
-        <v>3</v>
-      </c>
+      <c r="L185" s="51"/>
       <c r="M185" s="51"/>
       <c r="N185" s="49"/>
       <c r="O185">
@@ -7598,7 +7598,7 @@
       </c>
     </row>
     <row r="186" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A186" s="68"/>
+      <c r="A186" s="95"/>
       <c r="B186" s="38" t="s">
         <v>5</v>
       </c>
@@ -7608,7 +7608,7 @@
       </c>
       <c r="D186" s="44">
         <f t="shared" si="30"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E186" s="50"/>
       <c r="F186" s="51"/>
@@ -7618,9 +7618,7 @@
       <c r="J186" s="51"/>
       <c r="K186" s="51"/>
       <c r="L186" s="51"/>
-      <c r="M186" s="51">
-        <v>4</v>
-      </c>
+      <c r="M186" s="51"/>
       <c r="N186" s="49"/>
       <c r="O186">
         <v>17</v>
@@ -7630,7 +7628,7 @@
       </c>
     </row>
     <row r="187" spans="1:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A187" s="69"/>
+      <c r="A187" s="96"/>
       <c r="B187" s="40" t="s">
         <v>6</v>
       </c>
@@ -7640,7 +7638,7 @@
       </c>
       <c r="D187" s="44">
         <f t="shared" si="30"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E187" s="58"/>
       <c r="F187" s="59"/>
@@ -7650,9 +7648,7 @@
       <c r="J187" s="59"/>
       <c r="K187" s="59"/>
       <c r="L187" s="59"/>
-      <c r="M187" s="59">
-        <v>4</v>
-      </c>
+      <c r="M187" s="59"/>
       <c r="N187" s="49"/>
       <c r="O187">
         <v>18</v>
@@ -7662,7 +7658,7 @@
       </c>
     </row>
     <row r="188" spans="1:16" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A188" s="67" t="s">
+      <c r="A188" s="94" t="s">
         <v>59</v>
       </c>
       <c r="B188" s="38" t="s">
@@ -7674,7 +7670,7 @@
       </c>
       <c r="D188" s="44">
         <f t="shared" ref="D188:D194" si="32">SUM(E188:M188)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E188" s="56"/>
       <c r="F188" s="57"/>
@@ -7684,9 +7680,7 @@
       <c r="J188" s="57"/>
       <c r="K188" s="57"/>
       <c r="L188" s="57"/>
-      <c r="M188" s="57">
-        <v>2</v>
-      </c>
+      <c r="M188" s="57"/>
       <c r="N188" s="49"/>
       <c r="O188">
         <v>19</v>
@@ -7696,7 +7690,7 @@
       </c>
     </row>
     <row r="189" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A189" s="68"/>
+      <c r="A189" s="95"/>
       <c r="B189" s="38" t="s">
         <v>1</v>
       </c>
@@ -7706,7 +7700,7 @@
       </c>
       <c r="D189" s="44">
         <f t="shared" si="32"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E189" s="50"/>
       <c r="F189" s="51"/>
@@ -7716,9 +7710,7 @@
       <c r="J189" s="51"/>
       <c r="K189" s="51"/>
       <c r="L189" s="51"/>
-      <c r="M189" s="51">
-        <v>2</v>
-      </c>
+      <c r="M189" s="51"/>
       <c r="N189" s="49"/>
       <c r="O189">
         <v>20</v>
@@ -7728,7 +7720,7 @@
       </c>
     </row>
     <row r="190" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A190" s="68"/>
+      <c r="A190" s="95"/>
       <c r="B190" s="38" t="s">
         <v>2</v>
       </c>
@@ -7738,7 +7730,7 @@
       </c>
       <c r="D190" s="44">
         <f t="shared" si="32"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E190" s="50"/>
       <c r="F190" s="51"/>
@@ -7748,9 +7740,7 @@
       <c r="J190" s="51"/>
       <c r="K190" s="51"/>
       <c r="L190" s="51"/>
-      <c r="M190" s="51">
-        <v>3</v>
-      </c>
+      <c r="M190" s="51"/>
       <c r="N190" s="49"/>
       <c r="O190">
         <v>21</v>
@@ -7760,7 +7750,7 @@
       </c>
     </row>
     <row r="191" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A191" s="68"/>
+      <c r="A191" s="95"/>
       <c r="B191" s="38" t="s">
         <v>3</v>
       </c>
@@ -7770,7 +7760,7 @@
       </c>
       <c r="D191" s="44">
         <f t="shared" si="32"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E191" s="50"/>
       <c r="F191" s="51"/>
@@ -7780,9 +7770,7 @@
       <c r="J191" s="51"/>
       <c r="K191" s="51"/>
       <c r="L191" s="51"/>
-      <c r="M191" s="51">
-        <v>3</v>
-      </c>
+      <c r="M191" s="51"/>
       <c r="N191" s="49"/>
       <c r="O191">
         <v>22</v>
@@ -7792,7 +7780,7 @@
       </c>
     </row>
     <row r="192" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A192" s="68"/>
+      <c r="A192" s="95"/>
       <c r="B192" s="38" t="s">
         <v>4</v>
       </c>
@@ -7802,7 +7790,7 @@
       </c>
       <c r="D192" s="44">
         <f t="shared" si="32"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E192" s="50"/>
       <c r="F192" s="51"/>
@@ -7812,9 +7800,7 @@
       <c r="J192" s="51"/>
       <c r="K192" s="51"/>
       <c r="L192" s="51"/>
-      <c r="M192" s="51">
-        <v>3</v>
-      </c>
+      <c r="M192" s="51"/>
       <c r="N192" s="49"/>
       <c r="O192">
         <v>23</v>
@@ -7824,7 +7810,7 @@
       </c>
     </row>
     <row r="193" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A193" s="68"/>
+      <c r="A193" s="95"/>
       <c r="B193" s="38" t="s">
         <v>5</v>
       </c>
@@ -7834,7 +7820,7 @@
       </c>
       <c r="D193" s="44">
         <f t="shared" si="32"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E193" s="50"/>
       <c r="F193" s="51"/>
@@ -7844,9 +7830,7 @@
       <c r="J193" s="51"/>
       <c r="K193" s="51"/>
       <c r="L193" s="51"/>
-      <c r="M193" s="51">
-        <v>2</v>
-      </c>
+      <c r="M193" s="51"/>
       <c r="N193" s="49"/>
       <c r="O193">
         <v>24</v>
@@ -7856,7 +7840,7 @@
       </c>
     </row>
     <row r="194" spans="1:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A194" s="69"/>
+      <c r="A194" s="96"/>
       <c r="B194" s="40" t="s">
         <v>6</v>
       </c>
@@ -7886,7 +7870,7 @@
       </c>
     </row>
     <row r="195" spans="1:16" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A195" s="67" t="s">
+      <c r="A195" s="94" t="s">
         <v>59</v>
       </c>
       <c r="B195" s="38" t="s">
@@ -7898,7 +7882,7 @@
       </c>
       <c r="D195" s="44">
         <f t="shared" ref="D195:D201" si="34">SUM(E195:M195)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E195" s="56"/>
       <c r="F195" s="57"/>
@@ -7908,9 +7892,7 @@
       <c r="J195" s="57"/>
       <c r="K195" s="57"/>
       <c r="L195" s="57"/>
-      <c r="M195" s="57">
-        <v>5</v>
-      </c>
+      <c r="M195" s="57"/>
       <c r="N195" s="49"/>
       <c r="O195">
         <v>26</v>
@@ -7920,7 +7902,7 @@
       </c>
     </row>
     <row r="196" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A196" s="68"/>
+      <c r="A196" s="95"/>
       <c r="B196" s="38" t="s">
         <v>1</v>
       </c>
@@ -7930,7 +7912,7 @@
       </c>
       <c r="D196" s="44">
         <f t="shared" si="34"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E196" s="50"/>
       <c r="F196" s="51"/>
@@ -7940,9 +7922,7 @@
       <c r="J196" s="51"/>
       <c r="K196" s="51"/>
       <c r="L196" s="51"/>
-      <c r="M196" s="51">
-        <v>5</v>
-      </c>
+      <c r="M196" s="51"/>
       <c r="N196" s="49"/>
       <c r="O196">
         <v>27</v>
@@ -7952,7 +7932,7 @@
       </c>
     </row>
     <row r="197" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A197" s="68"/>
+      <c r="A197" s="95"/>
       <c r="B197" s="38" t="s">
         <v>2</v>
       </c>
@@ -7962,7 +7942,7 @@
       </c>
       <c r="D197" s="44">
         <f t="shared" si="34"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E197" s="50"/>
       <c r="F197" s="51"/>
@@ -7972,9 +7952,7 @@
       <c r="J197" s="51"/>
       <c r="K197" s="51"/>
       <c r="L197" s="51"/>
-      <c r="M197" s="51">
-        <v>5</v>
-      </c>
+      <c r="M197" s="51"/>
       <c r="N197" s="49"/>
       <c r="O197">
         <v>28</v>
@@ -7984,7 +7962,7 @@
       </c>
     </row>
     <row r="198" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A198" s="68"/>
+      <c r="A198" s="95"/>
       <c r="B198" s="38" t="s">
         <v>3</v>
       </c>
@@ -7994,7 +7972,7 @@
       </c>
       <c r="D198" s="44">
         <f t="shared" si="34"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E198" s="50"/>
       <c r="F198" s="51"/>
@@ -8004,9 +7982,7 @@
       <c r="J198" s="51"/>
       <c r="K198" s="51"/>
       <c r="L198" s="51"/>
-      <c r="M198" s="51">
-        <v>5</v>
-      </c>
+      <c r="M198" s="51"/>
       <c r="N198" s="49"/>
       <c r="O198">
         <v>29</v>
@@ -8016,7 +7992,7 @@
       </c>
     </row>
     <row r="199" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A199" s="68"/>
+      <c r="A199" s="95"/>
       <c r="B199" s="38" t="s">
         <v>4</v>
       </c>
@@ -8026,7 +8002,7 @@
       </c>
       <c r="D199" s="44">
         <f t="shared" si="34"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E199" s="50"/>
       <c r="F199" s="51"/>
@@ -8036,9 +8012,7 @@
       <c r="J199" s="51"/>
       <c r="K199" s="51"/>
       <c r="L199" s="51"/>
-      <c r="M199" s="51">
-        <v>5</v>
-      </c>
+      <c r="M199" s="51"/>
       <c r="N199" s="49"/>
       <c r="O199">
         <v>30</v>
@@ -8048,7 +8022,7 @@
       </c>
     </row>
     <row r="200" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A200" s="68"/>
+      <c r="A200" s="95"/>
       <c r="B200" s="38" t="s">
         <v>5</v>
       </c>
@@ -8058,7 +8032,7 @@
       </c>
       <c r="D200" s="44">
         <f t="shared" si="34"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E200" s="50"/>
       <c r="F200" s="51"/>
@@ -8068,9 +8042,7 @@
       <c r="J200" s="51"/>
       <c r="K200" s="51"/>
       <c r="L200" s="51"/>
-      <c r="M200" s="51">
-        <v>2</v>
-      </c>
+      <c r="M200" s="51"/>
       <c r="N200" s="49"/>
       <c r="O200">
         <v>31</v>
@@ -8080,7 +8052,7 @@
       </c>
     </row>
     <row r="201" spans="1:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A201" s="69"/>
+      <c r="A201" s="96"/>
       <c r="B201" s="40" t="s">
         <v>6</v>
       </c>
@@ -8922,22 +8894,22 @@
     <protectedRange sqref="E4:W5" name="Horas_libres"/>
   </protectedRanges>
   <mergeCells count="43">
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C1:R1"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:K2"/>
-    <mergeCell ref="L2:W2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="N20:N42"/>
-    <mergeCell ref="A27:A33"/>
-    <mergeCell ref="A34:A40"/>
-    <mergeCell ref="A41:A47"/>
-    <mergeCell ref="E5:W5"/>
-    <mergeCell ref="C7:E8"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="C10:K10"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="A167:A173"/>
+    <mergeCell ref="A174:A180"/>
+    <mergeCell ref="A181:A187"/>
+    <mergeCell ref="A188:A194"/>
+    <mergeCell ref="A195:A201"/>
+    <mergeCell ref="A160:A166"/>
+    <mergeCell ref="A90:A96"/>
+    <mergeCell ref="A97:A103"/>
+    <mergeCell ref="A104:A110"/>
+    <mergeCell ref="A111:A117"/>
+    <mergeCell ref="A118:A124"/>
+    <mergeCell ref="A125:A131"/>
+    <mergeCell ref="A132:A138"/>
+    <mergeCell ref="A139:A145"/>
+    <mergeCell ref="A146:A152"/>
+    <mergeCell ref="A153:A159"/>
     <mergeCell ref="A83:A89"/>
     <mergeCell ref="C14:D14"/>
     <mergeCell ref="C15:D15"/>
@@ -8949,22 +8921,22 @@
     <mergeCell ref="A62:A68"/>
     <mergeCell ref="A69:A75"/>
     <mergeCell ref="A76:A82"/>
-    <mergeCell ref="A160:A166"/>
-    <mergeCell ref="A90:A96"/>
-    <mergeCell ref="A97:A103"/>
-    <mergeCell ref="A104:A110"/>
-    <mergeCell ref="A111:A117"/>
-    <mergeCell ref="A118:A124"/>
-    <mergeCell ref="A125:A131"/>
-    <mergeCell ref="A132:A138"/>
-    <mergeCell ref="A139:A145"/>
-    <mergeCell ref="A146:A152"/>
-    <mergeCell ref="A153:A159"/>
-    <mergeCell ref="A167:A173"/>
-    <mergeCell ref="A174:A180"/>
-    <mergeCell ref="A181:A187"/>
-    <mergeCell ref="A188:A194"/>
-    <mergeCell ref="A195:A201"/>
+    <mergeCell ref="N20:N42"/>
+    <mergeCell ref="A27:A33"/>
+    <mergeCell ref="A34:A40"/>
+    <mergeCell ref="A41:A47"/>
+    <mergeCell ref="E5:W5"/>
+    <mergeCell ref="C7:E8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="C10:K10"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C1:R1"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:K2"/>
+    <mergeCell ref="L2:W2"/>
+    <mergeCell ref="C3:D3"/>
   </mergeCells>
   <phoneticPr fontId="31" type="noConversion"/>
   <conditionalFormatting sqref="D20:D61">

</xml_diff>